<commit_message>
Corrections of results process and further improvement of profile updating
</commit_message>
<xml_diff>
--- a/test-data.xlsx
+++ b/test-data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18675" windowHeight="9750" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18675" windowHeight="9750"/>
   </bookViews>
   <sheets>
     <sheet name="Divisions" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="32">
   <si>
     <t>Division 1</t>
   </si>
@@ -93,7 +93,34 @@
     <t>Fri 13</t>
   </si>
   <si>
-    <t>Mon 9</t>
+    <t>Etsuko Alleman</t>
+  </si>
+  <si>
+    <t>Brenton Vasko</t>
+  </si>
+  <si>
+    <t>Lenita Kerns</t>
+  </si>
+  <si>
+    <t>Wilburn Tebo</t>
+  </si>
+  <si>
+    <t>Elane Easterlington</t>
+  </si>
+  <si>
+    <t>Karrie Mahler</t>
+  </si>
+  <si>
+    <t>Thu 12</t>
+  </si>
+  <si>
+    <t>Sat 14</t>
+  </si>
+  <si>
+    <t>Tue 10</t>
+  </si>
+  <si>
+    <t>Mon 16</t>
   </si>
 </sst>
 </file>
@@ -231,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -272,6 +299,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -552,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,7 +595,7 @@
     <col min="8" max="8" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -572,7 +603,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -595,22 +626,25 @@
         <v>1</v>
       </c>
       <c r="I2" s="9">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J2" s="9">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="K2" s="9">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="L2" s="9">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="M2" s="9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="N2" s="20">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="10">
         <v>1</v>
       </c>
@@ -630,15 +664,28 @@
         <v>3</v>
       </c>
       <c r="H3" s="10">
-        <v>1</v>
-      </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="4"/>
-    </row>
-    <row r="4" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="14">
+        <v>1</v>
+      </c>
+      <c r="K3" s="14">
+        <v>3</v>
+      </c>
+      <c r="L3" s="14">
+        <v>2</v>
+      </c>
+      <c r="M3" s="15">
+        <v>0</v>
+      </c>
+      <c r="N3" s="17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="11">
         <v>2</v>
       </c>
@@ -658,15 +705,28 @@
         <v>2</v>
       </c>
       <c r="H4" s="11">
-        <v>2</v>
-      </c>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="6"/>
-    </row>
-    <row r="5" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="I4" s="16">
+        <v>1</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="16">
+        <v>2</v>
+      </c>
+      <c r="L4" s="16">
+        <v>0</v>
+      </c>
+      <c r="M4" s="17">
+        <v>3</v>
+      </c>
+      <c r="N4" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="11">
         <v>3</v>
       </c>
@@ -686,15 +746,28 @@
         <v>3</v>
       </c>
       <c r="H5" s="11">
-        <v>3</v>
-      </c>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="6"/>
-    </row>
-    <row r="6" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="I5" s="16">
+        <v>0</v>
+      </c>
+      <c r="J5" s="16">
+        <v>2</v>
+      </c>
+      <c r="K5" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="L5" s="16">
+        <v>1</v>
+      </c>
+      <c r="M5" s="17">
+        <v>3</v>
+      </c>
+      <c r="N5" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="11">
         <v>4</v>
       </c>
@@ -714,15 +787,28 @@
         <v>1</v>
       </c>
       <c r="H6" s="11">
-        <v>4</v>
-      </c>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="6"/>
-    </row>
-    <row r="7" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="I6" s="16">
+        <v>3</v>
+      </c>
+      <c r="J6" s="16">
+        <v>3</v>
+      </c>
+      <c r="K6" s="16">
+        <v>2</v>
+      </c>
+      <c r="L6" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="M6" s="17">
+        <v>3</v>
+      </c>
+      <c r="N6" s="17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>5</v>
       </c>
@@ -742,199 +828,342 @@
         <v>2</v>
       </c>
       <c r="H7" s="11">
-        <v>5</v>
-      </c>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="6"/>
-    </row>
-    <row r="8" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="I7" s="16">
+        <v>3</v>
+      </c>
+      <c r="J7" s="16">
+        <v>1</v>
+      </c>
+      <c r="K7" s="16">
+        <v>1</v>
+      </c>
+      <c r="L7" s="16">
+        <v>1</v>
+      </c>
+      <c r="M7" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="N7" s="17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="H8" s="12">
-        <v>6</v>
-      </c>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="8"/>
-    </row>
-    <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="18">
+        <v>0</v>
+      </c>
+      <c r="J8" s="18">
+        <v>2</v>
+      </c>
+      <c r="K8" s="18">
+        <v>3</v>
+      </c>
+      <c r="L8" s="18">
+        <v>0</v>
+      </c>
+      <c r="M8" s="19">
+        <v>3</v>
+      </c>
+      <c r="N8" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="H9" s="21"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+    </row>
+    <row r="11" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
+      <c r="H11" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="I12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="2">
-        <v>4</v>
-      </c>
-      <c r="C12" s="2">
-        <v>3</v>
-      </c>
-      <c r="D12" s="2">
-        <v>0</v>
-      </c>
-      <c r="E12" s="2">
-        <v>1</v>
-      </c>
-      <c r="F12" s="2">
+      <c r="B13" s="2">
+        <v>4</v>
+      </c>
+      <c r="C13" s="2">
+        <v>3</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="H13" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" s="2">
+        <v>5</v>
+      </c>
+      <c r="J13" s="13">
+        <v>2</v>
+      </c>
+      <c r="K13" s="13">
+        <v>1</v>
+      </c>
+      <c r="L13" s="13">
+        <v>2</v>
+      </c>
+      <c r="M13" s="13">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="2">
-        <v>4</v>
-      </c>
-      <c r="C13" s="2">
-        <v>3</v>
-      </c>
-      <c r="D13" s="2">
-        <v>1</v>
-      </c>
-      <c r="E13" s="2">
-        <v>0</v>
-      </c>
-      <c r="F13" s="2">
+      <c r="B14" s="2">
+        <v>4</v>
+      </c>
+      <c r="C14" s="2">
+        <v>3</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="H14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" s="2">
+        <v>5</v>
+      </c>
+      <c r="J14" s="13">
+        <v>1</v>
+      </c>
+      <c r="K14" s="13">
+        <v>2</v>
+      </c>
+      <c r="L14" s="13">
+        <v>2</v>
+      </c>
+      <c r="M14" s="13">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="2">
-        <v>4</v>
-      </c>
-      <c r="C14" s="2">
-        <v>1</v>
-      </c>
-      <c r="D14" s="2">
-        <v>0</v>
-      </c>
-      <c r="E14" s="2">
-        <v>3</v>
-      </c>
-      <c r="F14" s="2">
+      <c r="B15" s="2">
+        <v>4</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2">
+        <v>3</v>
+      </c>
+      <c r="F15" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="H15" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" s="2">
+        <v>5</v>
+      </c>
+      <c r="J15" s="13">
+        <v>1</v>
+      </c>
+      <c r="K15" s="13">
+        <v>1</v>
+      </c>
+      <c r="L15" s="13">
+        <v>3</v>
+      </c>
+      <c r="M15" s="13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="2">
-        <v>4</v>
-      </c>
-      <c r="C15" s="2">
-        <v>2</v>
-      </c>
-      <c r="D15" s="2">
-        <v>0</v>
-      </c>
-      <c r="E15" s="2">
-        <v>2</v>
-      </c>
-      <c r="F15" s="2">
+      <c r="B16" s="2">
+        <v>4</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2">
+        <v>3</v>
+      </c>
+      <c r="F16" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="H16" t="s">
+        <v>25</v>
+      </c>
+      <c r="I16" s="2">
+        <v>5</v>
+      </c>
+      <c r="J16" s="13">
+        <v>5</v>
+      </c>
+      <c r="K16" s="13">
+        <v>0</v>
+      </c>
+      <c r="L16" s="13">
+        <v>0</v>
+      </c>
+      <c r="M16" s="13">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="2">
-        <v>4</v>
-      </c>
-      <c r="C16" s="2">
-        <v>0</v>
-      </c>
-      <c r="D16" s="2">
-        <v>1</v>
-      </c>
-      <c r="E16" s="2">
-        <v>3</v>
-      </c>
-      <c r="F16" s="2">
+      <c r="B17" s="2">
+        <v>4</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2">
+        <v>2</v>
+      </c>
+      <c r="F17" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19" s="9">
-        <v>1</v>
-      </c>
-      <c r="C19" s="9">
-        <v>2</v>
-      </c>
-      <c r="D19" s="9">
-        <v>3</v>
-      </c>
-      <c r="E19" s="9">
-        <v>4</v>
-      </c>
-      <c r="F19" s="9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A20" s="10">
-        <v>1</v>
-      </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="4"/>
-    </row>
-    <row r="21" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="11">
-        <v>2</v>
-      </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="6"/>
-    </row>
-    <row r="22" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="11">
-        <v>3</v>
-      </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="6"/>
-    </row>
-    <row r="23" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="H17" t="s">
+        <v>26</v>
+      </c>
+      <c r="I17" s="2">
+        <v>5</v>
+      </c>
+      <c r="J17" s="13">
+        <v>1</v>
+      </c>
+      <c r="K17" s="13">
+        <v>0</v>
+      </c>
+      <c r="L17" s="13">
+        <v>4</v>
+      </c>
+      <c r="M17" s="13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>27</v>
+      </c>
+      <c r="I18" s="2">
+        <v>5</v>
+      </c>
+      <c r="J18" s="13">
+        <v>3</v>
+      </c>
+      <c r="K18" s="13">
+        <v>0</v>
+      </c>
+      <c r="L18" s="13">
+        <v>2</v>
+      </c>
+      <c r="M18" s="13">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="9">
+        <v>1</v>
+      </c>
+      <c r="C21" s="9">
+        <v>2</v>
+      </c>
+      <c r="D21" s="9">
+        <v>3</v>
+      </c>
+      <c r="E21" s="9">
+        <v>4</v>
+      </c>
+      <c r="F21" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A22" s="10">
+        <v>1</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="11">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -942,15 +1171,35 @@
       <c r="E23" s="5"/>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A24" s="12">
-        <v>5</v>
-      </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="8"/>
+    <row r="24" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A24" s="11">
+        <v>3</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="6"/>
+    </row>
+    <row r="25" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A25" s="11">
+        <v>4</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="6"/>
+    </row>
+    <row r="26" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A26" s="12">
+        <v>5</v>
+      </c>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -960,10 +1209,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1022,7 +1271,7 @@
         <v>75</v>
       </c>
       <c r="H2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1127,6 +1376,162 @@
       </c>
       <c r="H6" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>40</v>
+      </c>
+      <c r="H7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>20</v>
+      </c>
+      <c r="H8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+      <c r="G9">
+        <v>20</v>
+      </c>
+      <c r="H9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>100</v>
+      </c>
+      <c r="H10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+      <c r="G11">
+        <v>20</v>
+      </c>
+      <c r="H11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>60</v>
+      </c>
+      <c r="H12" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Solved issues with Updating Profiles code
</commit_message>
<xml_diff>
--- a/test-data.xlsx
+++ b/test-data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18675" windowHeight="9750"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18675" windowHeight="9750" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Divisions" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="39">
   <si>
     <t>Division 1</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Division 2</t>
   </si>
   <si>
-    <t>Rank</t>
-  </si>
-  <si>
     <t>Player</t>
   </si>
   <si>
@@ -121,6 +118,30 @@
   </si>
   <si>
     <t>Mon 16</t>
+  </si>
+  <si>
+    <t>Division 3</t>
+  </si>
+  <si>
+    <t>Clementine Jamal</t>
+  </si>
+  <si>
+    <t>Berneice Zebrowski</t>
+  </si>
+  <si>
+    <t>Libby Green</t>
+  </si>
+  <si>
+    <t>Dann Emberton</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Libby Geren</t>
+  </si>
+  <si>
+    <t>Wed 11</t>
   </si>
 </sst>
 </file>
@@ -166,7 +187,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -254,11 +275,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -303,6 +339,26 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -583,27 +639,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:U26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="U17" sqref="U17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
     <col min="8" max="8" width="17.85546875" customWidth="1"/>
+    <col min="16" max="16" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="P1" s="23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -643,9 +703,24 @@
       <c r="N2" s="20">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="10">
+      <c r="P2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="27">
+        <v>13</v>
+      </c>
+      <c r="R2" s="27">
+        <v>14</v>
+      </c>
+      <c r="S2" s="27">
+        <v>15</v>
+      </c>
+      <c r="T2" s="27">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="24">
         <v>1</v>
       </c>
       <c r="B3" s="14" t="s">
@@ -663,7 +738,7 @@
       <c r="F3" s="15">
         <v>3</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3" s="24">
         <v>6</v>
       </c>
       <c r="I3" s="14" t="s">
@@ -684,9 +759,24 @@
       <c r="N3" s="17">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="11">
+      <c r="P3" s="28">
+        <v>13</v>
+      </c>
+      <c r="Q3" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="R3" s="29">
+        <v>3</v>
+      </c>
+      <c r="S3" s="29">
+        <v>2</v>
+      </c>
+      <c r="T3" s="29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="25">
         <v>2</v>
       </c>
       <c r="B4" s="16">
@@ -704,7 +794,7 @@
       <c r="F4" s="17">
         <v>2</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="25">
         <v>7</v>
       </c>
       <c r="I4" s="16">
@@ -725,9 +815,24 @@
       <c r="N4" s="17">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="11">
+      <c r="P4" s="28">
+        <v>14</v>
+      </c>
+      <c r="Q4" s="29">
+        <v>0</v>
+      </c>
+      <c r="R4" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="S4" s="29">
+        <v>3</v>
+      </c>
+      <c r="T4" s="29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="25">
         <v>3</v>
       </c>
       <c r="B5" s="16">
@@ -745,7 +850,7 @@
       <c r="F5" s="17">
         <v>3</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="25">
         <v>8</v>
       </c>
       <c r="I5" s="16">
@@ -766,9 +871,24 @@
       <c r="N5" s="17">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="11">
+      <c r="P5" s="28">
+        <v>15</v>
+      </c>
+      <c r="Q5" s="29">
+        <v>1</v>
+      </c>
+      <c r="R5" s="29">
+        <v>1</v>
+      </c>
+      <c r="S5" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="T5" s="29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="25">
         <v>4</v>
       </c>
       <c r="B6" s="16">
@@ -786,7 +906,7 @@
       <c r="F6" s="17">
         <v>1</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="25">
         <v>9</v>
       </c>
       <c r="I6" s="16">
@@ -807,9 +927,24 @@
       <c r="N6" s="17">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="12">
+      <c r="P6" s="28">
+        <v>16</v>
+      </c>
+      <c r="Q6" s="29">
+        <v>2</v>
+      </c>
+      <c r="R6" s="29">
+        <v>1</v>
+      </c>
+      <c r="S6" s="29">
+        <v>3</v>
+      </c>
+      <c r="T6" s="29" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="26">
         <v>5</v>
       </c>
       <c r="B7" s="18">
@@ -827,7 +962,7 @@
       <c r="F7" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="25">
         <v>10</v>
       </c>
       <c r="I7" s="16">
@@ -849,8 +984,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="H8" s="12">
+    <row r="8" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="H8" s="26">
         <v>11</v>
       </c>
       <c r="I8" s="18">
@@ -872,7 +1007,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="H9" s="21"/>
       <c r="I9" s="16"/>
       <c r="J9" s="16"/>
@@ -881,49 +1016,68 @@
       <c r="M9" s="16"/>
       <c r="N9" s="16"/>
     </row>
-    <row r="11" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="I12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M12" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
+      <c r="P12" s="22"/>
+      <c r="Q12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="R12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="S12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="T12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="U12" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="2">
         <v>4</v>
@@ -941,7 +1095,7 @@
         <v>17</v>
       </c>
       <c r="H13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I13" s="2">
         <v>5</v>
@@ -958,10 +1112,28 @@
       <c r="M13" s="13">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="P13" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>3</v>
+      </c>
+      <c r="R13" s="2">
+        <v>2</v>
+      </c>
+      <c r="S13" s="2">
+        <v>1</v>
+      </c>
+      <c r="T13" s="2">
+        <v>0</v>
+      </c>
+      <c r="U13" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="2">
         <v>4</v>
@@ -979,7 +1151,7 @@
         <v>16</v>
       </c>
       <c r="H14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I14" s="2">
         <v>5</v>
@@ -996,10 +1168,28 @@
       <c r="M14" s="13">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="P14" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>3</v>
+      </c>
+      <c r="R14" s="2">
+        <v>2</v>
+      </c>
+      <c r="S14" s="2">
+        <v>0</v>
+      </c>
+      <c r="T14" s="2">
+        <v>1</v>
+      </c>
+      <c r="U14" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" s="2">
         <v>4</v>
@@ -1017,7 +1207,7 @@
         <v>9</v>
       </c>
       <c r="H15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I15" s="2">
         <v>5</v>
@@ -1034,10 +1224,28 @@
       <c r="M15" s="13">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="P15" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>3</v>
+      </c>
+      <c r="R15" s="2">
+        <v>0</v>
+      </c>
+      <c r="S15" s="2">
+        <v>0</v>
+      </c>
+      <c r="T15" s="2">
+        <v>3</v>
+      </c>
+      <c r="U15" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="2">
         <v>4</v>
@@ -1055,7 +1263,7 @@
         <v>10</v>
       </c>
       <c r="H16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I16" s="2">
         <v>5</v>
@@ -1072,10 +1280,28 @@
       <c r="M16" s="13">
         <v>24</v>
       </c>
+      <c r="P16" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>3</v>
+      </c>
+      <c r="R16" s="2">
+        <v>1</v>
+      </c>
+      <c r="S16" s="2">
+        <v>1</v>
+      </c>
+      <c r="T16" s="2">
+        <v>1</v>
+      </c>
+      <c r="U16" s="2">
+        <v>9</v>
+      </c>
     </row>
     <row r="17" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="2">
         <v>4</v>
@@ -1093,7 +1319,7 @@
         <v>8</v>
       </c>
       <c r="H17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I17" s="2">
         <v>5</v>
@@ -1113,7 +1339,7 @@
     </row>
     <row r="18" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I18" s="2">
         <v>5</v>
@@ -1209,10 +1435,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1224,28 +1450,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="B1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="F1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>11</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1253,7 +1479,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2">
         <v>4</v>
@@ -1271,7 +1497,7 @@
         <v>75</v>
       </c>
       <c r="H2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1279,7 +1505,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3">
         <v>4</v>
@@ -1297,7 +1523,7 @@
         <v>75</v>
       </c>
       <c r="H3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1305,7 +1531,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4">
         <v>4</v>
@@ -1323,7 +1549,7 @@
         <v>25</v>
       </c>
       <c r="H4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1331,7 +1557,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -1349,7 +1575,7 @@
         <v>25</v>
       </c>
       <c r="H5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1357,7 +1583,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -1375,7 +1601,7 @@
         <v>25</v>
       </c>
       <c r="H6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1383,7 +1609,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -1401,7 +1627,7 @@
         <v>40</v>
       </c>
       <c r="H7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1409,7 +1635,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -1427,7 +1653,7 @@
         <v>20</v>
       </c>
       <c r="H8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1435,7 +1661,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9">
         <v>5</v>
@@ -1453,7 +1679,7 @@
         <v>20</v>
       </c>
       <c r="H9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1461,7 +1687,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -1479,7 +1705,7 @@
         <v>100</v>
       </c>
       <c r="H10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1487,7 +1713,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11">
         <v>5</v>
@@ -1505,7 +1731,7 @@
         <v>20</v>
       </c>
       <c r="H11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1513,7 +1739,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12">
         <v>5</v>
@@ -1531,7 +1757,111 @@
         <v>60</v>
       </c>
       <c r="H12" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>66.599999999999994</v>
+      </c>
+      <c r="H13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>66.599999999999994</v>
+      </c>
+      <c r="H14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>3</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="H16" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Amendments to profile update
</commit_message>
<xml_diff>
--- a/test-data.xlsx
+++ b/test-data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18675" windowHeight="9750" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18675" windowHeight="9750"/>
   </bookViews>
   <sheets>
     <sheet name="Divisions" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="58">
   <si>
     <t>Division 1</t>
   </si>
@@ -142,6 +142,63 @@
   </si>
   <si>
     <t>Wed 11</t>
+  </si>
+  <si>
+    <t>Division 4</t>
+  </si>
+  <si>
+    <t>Hildegard Perreault</t>
+  </si>
+  <si>
+    <t>Jennefer Ricotta</t>
+  </si>
+  <si>
+    <t>Bethanie Collom</t>
+  </si>
+  <si>
+    <t>Kellee Bea</t>
+  </si>
+  <si>
+    <t>Detra Edson</t>
+  </si>
+  <si>
+    <t>Wed 18</t>
+  </si>
+  <si>
+    <t>Fri 20</t>
+  </si>
+  <si>
+    <t>Division 5</t>
+  </si>
+  <si>
+    <t>Jesse Henriques</t>
+  </si>
+  <si>
+    <t>Keena Silvers</t>
+  </si>
+  <si>
+    <t>Oleta Fortuna</t>
+  </si>
+  <si>
+    <t>Arlyne Bodden</t>
+  </si>
+  <si>
+    <t>Seraphinia Hirano</t>
+  </si>
+  <si>
+    <t>Robert Squashy</t>
+  </si>
+  <si>
+    <t>Wed 25</t>
+  </si>
+  <si>
+    <t>Tue 24</t>
+  </si>
+  <si>
+    <t>Sat 28</t>
+  </si>
+  <si>
+    <t>Thu 26</t>
   </si>
 </sst>
 </file>
@@ -294,7 +351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -353,11 +410,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -639,10 +708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U26"/>
+  <dimension ref="A1:AI26"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="U17" sqref="U17"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AH18" sqref="AH18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,9 +719,11 @@
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
     <col min="8" max="8" width="17.85546875" customWidth="1"/>
     <col min="16" max="16" width="18.85546875" customWidth="1"/>
+    <col min="22" max="22" width="18.5703125" customWidth="1"/>
+    <col min="29" max="29" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -662,8 +733,14 @@
       <c r="P1" s="23" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="V1" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC1" s="23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -718,8 +795,47 @@
       <c r="T2" s="27">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="V2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" s="9">
+        <v>17</v>
+      </c>
+      <c r="X2" s="9">
+        <v>18</v>
+      </c>
+      <c r="Y2" s="9">
+        <v>19</v>
+      </c>
+      <c r="Z2" s="9">
+        <v>20</v>
+      </c>
+      <c r="AA2" s="9">
+        <v>21</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD2" s="9">
+        <v>22</v>
+      </c>
+      <c r="AE2" s="9">
+        <v>23</v>
+      </c>
+      <c r="AF2" s="9">
+        <v>24</v>
+      </c>
+      <c r="AG2" s="9">
+        <v>25</v>
+      </c>
+      <c r="AH2" s="9">
+        <v>26</v>
+      </c>
+      <c r="AI2" s="9">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="24">
         <v>1</v>
       </c>
@@ -759,23 +875,62 @@
       <c r="N3" s="17">
         <v>2</v>
       </c>
-      <c r="P3" s="28">
+      <c r="P3" s="29">
         <v>13</v>
       </c>
-      <c r="Q3" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="R3" s="29">
-        <v>3</v>
-      </c>
-      <c r="S3" s="29">
-        <v>2</v>
-      </c>
-      <c r="T3" s="29">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="Q3" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="R3" s="28">
+        <v>3</v>
+      </c>
+      <c r="S3" s="28">
+        <v>2</v>
+      </c>
+      <c r="T3" s="28">
+        <v>2</v>
+      </c>
+      <c r="V3" s="30">
+        <v>17</v>
+      </c>
+      <c r="W3" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="X3" s="28">
+        <v>3</v>
+      </c>
+      <c r="Y3" s="28">
+        <v>2</v>
+      </c>
+      <c r="Z3" s="28">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="28">
+        <v>3</v>
+      </c>
+      <c r="AC3" s="30">
+        <v>22</v>
+      </c>
+      <c r="AD3" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE3" s="28">
+        <v>2</v>
+      </c>
+      <c r="AF3" s="28">
+        <v>3</v>
+      </c>
+      <c r="AG3" s="28">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="28">
+        <v>1</v>
+      </c>
+      <c r="AI3" s="32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="25">
         <v>2</v>
       </c>
@@ -815,23 +970,62 @@
       <c r="N4" s="17">
         <v>1</v>
       </c>
-      <c r="P4" s="28">
+      <c r="P4" s="29">
         <v>14</v>
       </c>
-      <c r="Q4" s="29">
-        <v>0</v>
-      </c>
-      <c r="R4" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="S4" s="29">
-        <v>3</v>
-      </c>
-      <c r="T4" s="29">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="Q4" s="28">
+        <v>0</v>
+      </c>
+      <c r="R4" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="S4" s="28">
+        <v>3</v>
+      </c>
+      <c r="T4" s="28">
+        <v>2</v>
+      </c>
+      <c r="V4" s="30">
+        <v>18</v>
+      </c>
+      <c r="W4" s="28">
+        <v>1</v>
+      </c>
+      <c r="X4" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y4" s="28">
+        <v>2</v>
+      </c>
+      <c r="Z4" s="28">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="28">
+        <v>1</v>
+      </c>
+      <c r="AC4" s="30">
+        <v>23</v>
+      </c>
+      <c r="AD4" s="28">
+        <v>2</v>
+      </c>
+      <c r="AE4" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF4" s="28">
+        <v>1</v>
+      </c>
+      <c r="AG4" s="28">
+        <v>3</v>
+      </c>
+      <c r="AH4" s="28">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="25">
         <v>3</v>
       </c>
@@ -871,23 +1065,62 @@
       <c r="N5" s="17">
         <v>0</v>
       </c>
-      <c r="P5" s="28">
+      <c r="P5" s="29">
         <v>15</v>
       </c>
-      <c r="Q5" s="29">
-        <v>1</v>
-      </c>
-      <c r="R5" s="29">
-        <v>1</v>
-      </c>
-      <c r="S5" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="T5" s="29">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="Q5" s="28">
+        <v>1</v>
+      </c>
+      <c r="R5" s="28">
+        <v>1</v>
+      </c>
+      <c r="S5" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="T5" s="28">
+        <v>2</v>
+      </c>
+      <c r="V5" s="30">
+        <v>19</v>
+      </c>
+      <c r="W5" s="28">
+        <v>3</v>
+      </c>
+      <c r="X5" s="28">
+        <v>2</v>
+      </c>
+      <c r="Y5" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z5" s="28">
+        <v>3</v>
+      </c>
+      <c r="AA5" s="28">
+        <v>2</v>
+      </c>
+      <c r="AC5" s="30">
+        <v>24</v>
+      </c>
+      <c r="AD5" s="28">
+        <v>2</v>
+      </c>
+      <c r="AE5" s="28">
+        <v>2</v>
+      </c>
+      <c r="AF5" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG5" s="28">
+        <v>3</v>
+      </c>
+      <c r="AH5" s="28">
+        <v>0</v>
+      </c>
+      <c r="AI5" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="25">
         <v>4</v>
       </c>
@@ -927,23 +1160,62 @@
       <c r="N6" s="17">
         <v>2</v>
       </c>
-      <c r="P6" s="28">
+      <c r="P6" s="29">
         <v>16</v>
       </c>
-      <c r="Q6" s="29">
-        <v>2</v>
-      </c>
-      <c r="R6" s="29">
-        <v>1</v>
-      </c>
-      <c r="S6" s="29">
-        <v>3</v>
-      </c>
-      <c r="T6" s="29" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="Q6" s="28">
+        <v>2</v>
+      </c>
+      <c r="R6" s="28">
+        <v>1</v>
+      </c>
+      <c r="S6" s="28">
+        <v>3</v>
+      </c>
+      <c r="T6" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="V6" s="30">
+        <v>20</v>
+      </c>
+      <c r="W6" s="28">
+        <v>1</v>
+      </c>
+      <c r="X6" s="28">
+        <v>3</v>
+      </c>
+      <c r="Y6" s="28">
+        <v>2</v>
+      </c>
+      <c r="Z6" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA6" s="28">
+        <v>2</v>
+      </c>
+      <c r="AC6" s="30">
+        <v>25</v>
+      </c>
+      <c r="AD6" s="28">
+        <v>3</v>
+      </c>
+      <c r="AE6" s="28">
+        <v>1</v>
+      </c>
+      <c r="AF6" s="28">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH6" s="28">
+        <v>2</v>
+      </c>
+      <c r="AI6" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="26">
         <v>5</v>
       </c>
@@ -983,8 +1255,47 @@
       <c r="N7" s="17">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="V7" s="30">
+        <v>21</v>
+      </c>
+      <c r="W7" s="28">
+        <v>0</v>
+      </c>
+      <c r="X7" s="28">
+        <v>3</v>
+      </c>
+      <c r="Y7" s="28">
+        <v>3</v>
+      </c>
+      <c r="Z7" s="28">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC7" s="30">
+        <v>26</v>
+      </c>
+      <c r="AD7" s="28">
+        <v>3</v>
+      </c>
+      <c r="AE7" s="28">
+        <v>2</v>
+      </c>
+      <c r="AF7" s="28">
+        <v>3</v>
+      </c>
+      <c r="AG7" s="28">
+        <v>3</v>
+      </c>
+      <c r="AH7" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI7" s="32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" ht="18.75" x14ac:dyDescent="0.3">
       <c r="H8" s="26">
         <v>11</v>
       </c>
@@ -1006,8 +1317,29 @@
       <c r="N8" s="19" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AC8" s="29">
+        <v>29</v>
+      </c>
+      <c r="AD8" s="32">
+        <v>1</v>
+      </c>
+      <c r="AE8" s="32">
+        <v>2</v>
+      </c>
+      <c r="AF8" s="32">
+        <v>3</v>
+      </c>
+      <c r="AG8" s="32">
+        <v>1</v>
+      </c>
+      <c r="AH8" s="32">
+        <v>1</v>
+      </c>
+      <c r="AI8" s="32" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" ht="18.75" x14ac:dyDescent="0.3">
       <c r="H9" s="21"/>
       <c r="I9" s="16"/>
       <c r="J9" s="16"/>
@@ -1016,7 +1348,7 @@
       <c r="M9" s="16"/>
       <c r="N9" s="16"/>
     </row>
-    <row r="11" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -1026,8 +1358,24 @@
       <c r="P11" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="2"/>
+      <c r="AA11" s="2"/>
+      <c r="AC11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD11" s="2"/>
+      <c r="AE11" s="2"/>
+      <c r="AF11" s="2"/>
+      <c r="AG11" s="2"/>
+      <c r="AH11" s="2"/>
+    </row>
+    <row r="12" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>6</v>
       </c>
@@ -1074,8 +1422,40 @@
       <c r="U12" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V12" s="2"/>
+      <c r="W12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="X12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC12" s="2"/>
+      <c r="AD12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH12" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1130,8 +1510,44 @@
       <c r="U13" s="2">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="W13" s="2">
+        <v>4</v>
+      </c>
+      <c r="X13" s="2">
+        <v>2</v>
+      </c>
+      <c r="Y13" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z13" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA13" s="2">
+        <v>16</v>
+      </c>
+      <c r="AC13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD13" s="2">
+        <v>5</v>
+      </c>
+      <c r="AE13" s="2">
+        <v>2</v>
+      </c>
+      <c r="AF13" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG13" s="2">
+        <v>2</v>
+      </c>
+      <c r="AH13" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1186,8 +1602,44 @@
       <c r="U14" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="W14" s="2">
+        <v>4</v>
+      </c>
+      <c r="X14" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z14" s="2">
+        <v>3</v>
+      </c>
+      <c r="AA14" s="2">
+        <v>6</v>
+      </c>
+      <c r="AC14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD14" s="2">
+        <v>5</v>
+      </c>
+      <c r="AE14" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF14" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG14" s="2">
+        <v>3</v>
+      </c>
+      <c r="AH14" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1242,8 +1694,44 @@
       <c r="U15" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="W15" s="2">
+        <v>4</v>
+      </c>
+      <c r="X15" s="2">
+        <v>2</v>
+      </c>
+      <c r="Y15" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z15" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA15" s="2">
+        <v>13</v>
+      </c>
+      <c r="AC15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD15" s="2">
+        <v>5</v>
+      </c>
+      <c r="AE15" s="2">
+        <v>2</v>
+      </c>
+      <c r="AF15" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG15" s="2">
+        <v>3</v>
+      </c>
+      <c r="AH15" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1298,8 +1786,44 @@
       <c r="U16" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="W16" s="2">
+        <v>4</v>
+      </c>
+      <c r="X16" s="2">
+        <v>2</v>
+      </c>
+      <c r="Y16" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z16" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA16" s="2">
+        <v>14</v>
+      </c>
+      <c r="AC16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD16" s="2">
+        <v>5</v>
+      </c>
+      <c r="AE16" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF16" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG16" s="2">
+        <v>3</v>
+      </c>
+      <c r="AH16" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1336,8 +1860,44 @@
       <c r="M17" s="13">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="W17" s="2">
+        <v>4</v>
+      </c>
+      <c r="X17" s="2">
+        <v>2</v>
+      </c>
+      <c r="Y17" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="2">
+        <v>2</v>
+      </c>
+      <c r="AA17" s="2">
+        <v>11</v>
+      </c>
+      <c r="AC17" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD17" s="2">
+        <v>5</v>
+      </c>
+      <c r="AE17" s="2">
+        <v>5</v>
+      </c>
+      <c r="AF17" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG17" s="2">
+        <v>0</v>
+      </c>
+      <c r="AH17" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H18" t="s">
         <v>26</v>
       </c>
@@ -1356,8 +1916,26 @@
       <c r="M18" s="13">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AC18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD18" s="2">
+        <v>5</v>
+      </c>
+      <c r="AE18" s="2">
+        <v>2</v>
+      </c>
+      <c r="AF18" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG18" s="2">
+        <v>2</v>
+      </c>
+      <c r="AH18" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:34" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>3</v>
       </c>
@@ -1377,7 +1955,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:34" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="10">
         <v>1</v>
       </c>
@@ -1387,7 +1965,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:34" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="11">
         <v>2</v>
       </c>
@@ -1397,7 +1975,7 @@
       <c r="E23" s="5"/>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:34" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="11">
         <v>3</v>
       </c>
@@ -1407,7 +1985,7 @@
       <c r="E24" s="5"/>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:34" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="11">
         <v>4</v>
       </c>
@@ -1417,7 +1995,7 @@
       <c r="E25" s="5"/>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:34" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="12">
         <v>5</v>
       </c>
@@ -1435,15 +2013,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" style="33" customWidth="1"/>
     <col min="7" max="7" width="10.28515625" customWidth="1"/>
     <col min="8" max="8" width="13.42578125" customWidth="1"/>
   </cols>
@@ -1452,7 +2030,7 @@
       <c r="A1" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="33" t="s">
         <v>5</v>
       </c>
       <c r="C1" s="13" t="s">
@@ -1478,22 +2056,22 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="13">
         <v>4</v>
       </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
+      <c r="D2" s="13">
+        <v>3</v>
+      </c>
+      <c r="E2" s="13">
+        <v>0</v>
+      </c>
+      <c r="F2" s="13">
+        <v>1</v>
+      </c>
+      <c r="G2" s="13">
         <v>75</v>
       </c>
       <c r="H2" t="s">
@@ -1504,22 +2082,22 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="13">
         <v>4</v>
       </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
+      <c r="D3" s="13">
+        <v>3</v>
+      </c>
+      <c r="E3" s="13">
+        <v>1</v>
+      </c>
+      <c r="F3" s="13">
+        <v>0</v>
+      </c>
+      <c r="G3" s="13">
         <v>75</v>
       </c>
       <c r="H3" t="s">
@@ -1530,22 +2108,22 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="13">
         <v>4</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-      <c r="G4">
+      <c r="D4" s="13">
+        <v>1</v>
+      </c>
+      <c r="E4" s="13">
+        <v>0</v>
+      </c>
+      <c r="F4" s="13">
+        <v>3</v>
+      </c>
+      <c r="G4" s="13">
         <v>25</v>
       </c>
       <c r="H4" t="s">
@@ -1556,22 +2134,22 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="13">
         <v>4</v>
       </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>3</v>
-      </c>
-      <c r="G5">
+      <c r="D5" s="13">
+        <v>1</v>
+      </c>
+      <c r="E5" s="13">
+        <v>0</v>
+      </c>
+      <c r="F5" s="13">
+        <v>3</v>
+      </c>
+      <c r="G5" s="13">
         <v>25</v>
       </c>
       <c r="H5" t="s">
@@ -1582,22 +2160,22 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="13">
         <v>4</v>
       </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>2</v>
-      </c>
-      <c r="G6">
+      <c r="D6" s="13">
+        <v>1</v>
+      </c>
+      <c r="E6" s="13">
+        <v>1</v>
+      </c>
+      <c r="F6" s="13">
+        <v>2</v>
+      </c>
+      <c r="G6" s="13">
         <v>25</v>
       </c>
       <c r="H6" t="s">
@@ -1608,22 +2186,22 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="C7">
-        <v>5</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>2</v>
-      </c>
-      <c r="G7">
+      <c r="C7" s="13">
+        <v>5</v>
+      </c>
+      <c r="D7" s="13">
+        <v>2</v>
+      </c>
+      <c r="E7" s="13">
+        <v>1</v>
+      </c>
+      <c r="F7" s="13">
+        <v>2</v>
+      </c>
+      <c r="G7" s="13">
         <v>40</v>
       </c>
       <c r="H7" t="s">
@@ -1634,22 +2212,22 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="C8">
-        <v>5</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
-      <c r="F8">
-        <v>2</v>
-      </c>
-      <c r="G8">
+      <c r="C8" s="13">
+        <v>5</v>
+      </c>
+      <c r="D8" s="13">
+        <v>1</v>
+      </c>
+      <c r="E8" s="13">
+        <v>2</v>
+      </c>
+      <c r="F8" s="13">
+        <v>2</v>
+      </c>
+      <c r="G8" s="13">
         <v>20</v>
       </c>
       <c r="H8" t="s">
@@ -1660,22 +2238,22 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="C9">
-        <v>5</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>3</v>
-      </c>
-      <c r="G9">
+      <c r="C9" s="13">
+        <v>5</v>
+      </c>
+      <c r="D9" s="13">
+        <v>1</v>
+      </c>
+      <c r="E9" s="13">
+        <v>1</v>
+      </c>
+      <c r="F9" s="13">
+        <v>3</v>
+      </c>
+      <c r="G9" s="13">
         <v>20</v>
       </c>
       <c r="H9" t="s">
@@ -1686,22 +2264,22 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="C10">
-        <v>5</v>
-      </c>
-      <c r="D10">
-        <v>5</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
+      <c r="C10" s="13">
+        <v>5</v>
+      </c>
+      <c r="D10" s="13">
+        <v>5</v>
+      </c>
+      <c r="E10" s="13">
+        <v>0</v>
+      </c>
+      <c r="F10" s="13">
+        <v>0</v>
+      </c>
+      <c r="G10" s="13">
         <v>100</v>
       </c>
       <c r="H10" t="s">
@@ -1712,22 +2290,22 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="C11">
-        <v>5</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
+      <c r="C11" s="13">
+        <v>5</v>
+      </c>
+      <c r="D11" s="13">
+        <v>1</v>
+      </c>
+      <c r="E11" s="13">
+        <v>0</v>
+      </c>
+      <c r="F11" s="13">
         <v>4</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="13">
         <v>20</v>
       </c>
       <c r="H11" t="s">
@@ -1738,22 +2316,22 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="C12">
-        <v>5</v>
-      </c>
-      <c r="D12">
-        <v>3</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>2</v>
-      </c>
-      <c r="G12">
+      <c r="C12" s="13">
+        <v>5</v>
+      </c>
+      <c r="D12" s="13">
+        <v>3</v>
+      </c>
+      <c r="E12" s="13">
+        <v>0</v>
+      </c>
+      <c r="F12" s="13">
+        <v>2</v>
+      </c>
+      <c r="G12" s="13">
         <v>60</v>
       </c>
       <c r="H12" t="s">
@@ -1764,23 +2342,23 @@
       <c r="A13">
         <v>13</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="C13">
-        <v>3</v>
-      </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>66.599999999999994</v>
+      <c r="C13" s="13">
+        <v>3</v>
+      </c>
+      <c r="D13" s="13">
+        <v>2</v>
+      </c>
+      <c r="E13" s="13">
+        <v>1</v>
+      </c>
+      <c r="F13" s="13">
+        <v>0</v>
+      </c>
+      <c r="G13" s="13">
+        <v>66.7</v>
       </c>
       <c r="H13" t="s">
         <v>38</v>
@@ -1790,23 +2368,23 @@
       <c r="A14">
         <v>14</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="C14">
-        <v>3</v>
-      </c>
-      <c r="D14">
-        <v>2</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14">
-        <v>66.599999999999994</v>
+      <c r="C14" s="13">
+        <v>3</v>
+      </c>
+      <c r="D14" s="13">
+        <v>2</v>
+      </c>
+      <c r="E14" s="13">
+        <v>0</v>
+      </c>
+      <c r="F14" s="13">
+        <v>1</v>
+      </c>
+      <c r="G14" s="13">
+        <v>66.7</v>
       </c>
       <c r="H14" t="s">
         <v>20</v>
@@ -1816,22 +2394,22 @@
       <c r="A15">
         <v>15</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="C15">
-        <v>3</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>3</v>
-      </c>
-      <c r="G15">
+      <c r="C15" s="13">
+        <v>3</v>
+      </c>
+      <c r="D15" s="13">
+        <v>0</v>
+      </c>
+      <c r="E15" s="13">
+        <v>0</v>
+      </c>
+      <c r="F15" s="13">
+        <v>3</v>
+      </c>
+      <c r="G15" s="13">
         <v>0</v>
       </c>
       <c r="H15" t="s">
@@ -1842,26 +2420,312 @@
       <c r="A16">
         <v>16</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="C16">
-        <v>3</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16">
+      <c r="C16" s="13">
+        <v>3</v>
+      </c>
+      <c r="D16" s="13">
+        <v>1</v>
+      </c>
+      <c r="E16" s="13">
+        <v>1</v>
+      </c>
+      <c r="F16" s="13">
+        <v>1</v>
+      </c>
+      <c r="G16" s="13">
         <v>33.299999999999997</v>
       </c>
       <c r="H16" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="13">
+        <v>4</v>
+      </c>
+      <c r="D17" s="2">
+        <v>2</v>
+      </c>
+      <c r="E17" s="2">
+        <v>1</v>
+      </c>
+      <c r="F17" s="2">
+        <v>1</v>
+      </c>
+      <c r="G17" s="2">
+        <v>50</v>
+      </c>
+      <c r="H17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="13">
+        <v>4</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2">
+        <v>1</v>
+      </c>
+      <c r="F18" s="2">
+        <v>3</v>
+      </c>
+      <c r="G18" s="13">
+        <v>0</v>
+      </c>
+      <c r="H18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="13">
+        <v>4</v>
+      </c>
+      <c r="D19" s="2">
+        <v>2</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1</v>
+      </c>
+      <c r="F19" s="2">
+        <v>1</v>
+      </c>
+      <c r="G19" s="13">
+        <v>50</v>
+      </c>
+      <c r="H19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="13">
+        <v>4</v>
+      </c>
+      <c r="D20" s="2">
+        <v>2</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1</v>
+      </c>
+      <c r="F20" s="2">
+        <v>1</v>
+      </c>
+      <c r="G20" s="13">
+        <v>50</v>
+      </c>
+      <c r="H20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="13">
+        <v>4</v>
+      </c>
+      <c r="D21" s="2">
+        <v>2</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0</v>
+      </c>
+      <c r="F21" s="2">
+        <v>2</v>
+      </c>
+      <c r="G21" s="13">
+        <v>50</v>
+      </c>
+      <c r="H21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="B22" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="2">
+        <v>5</v>
+      </c>
+      <c r="D22" s="2">
+        <v>2</v>
+      </c>
+      <c r="E22" s="2">
+        <v>1</v>
+      </c>
+      <c r="F22" s="2">
+        <v>2</v>
+      </c>
+      <c r="G22" s="13">
+        <v>40</v>
+      </c>
+      <c r="H22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="2">
+        <v>5</v>
+      </c>
+      <c r="D23" s="2">
+        <v>1</v>
+      </c>
+      <c r="E23" s="2">
+        <v>2</v>
+      </c>
+      <c r="F23" s="2">
+        <v>2</v>
+      </c>
+      <c r="G23" s="13">
+        <v>20</v>
+      </c>
+      <c r="H23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="B24" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="2">
+        <v>5</v>
+      </c>
+      <c r="D24" s="2">
+        <v>2</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0</v>
+      </c>
+      <c r="F24" s="2">
+        <v>3</v>
+      </c>
+      <c r="G24" s="13">
+        <v>40</v>
+      </c>
+      <c r="H24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="2">
+        <v>5</v>
+      </c>
+      <c r="D25" s="2">
+        <v>1</v>
+      </c>
+      <c r="E25" s="2">
+        <v>1</v>
+      </c>
+      <c r="F25" s="2">
+        <v>3</v>
+      </c>
+      <c r="G25" s="13">
+        <v>20</v>
+      </c>
+      <c r="H25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>26</v>
+      </c>
+      <c r="B26" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="2">
+        <v>5</v>
+      </c>
+      <c r="D26" s="2">
+        <v>5</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0</v>
+      </c>
+      <c r="G26" s="13">
+        <v>100</v>
+      </c>
+      <c r="H26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>29</v>
+      </c>
+      <c r="B27" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="2">
+        <v>5</v>
+      </c>
+      <c r="D27" s="2">
+        <v>2</v>
+      </c>
+      <c r="E27" s="2">
+        <v>1</v>
+      </c>
+      <c r="F27" s="2">
+        <v>2</v>
+      </c>
+      <c r="G27" s="13">
+        <v>40</v>
+      </c>
+      <c r="H27" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Further improvement of results initiation process and viewing of next month's divs by users
</commit_message>
<xml_diff>
--- a/test-data.xlsx
+++ b/test-data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="62">
   <si>
     <t>Division 1</t>
   </si>
@@ -256,7 +256,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -359,11 +359,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -447,6 +460,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -729,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ38"/>
+  <dimension ref="A1:AQ39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W11" workbookViewId="0">
-      <selection activeCell="AI25" sqref="AI25"/>
+    <sheetView tabSelected="1" topLeftCell="X11" workbookViewId="0">
+      <selection activeCell="AF25" sqref="AF25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1979,7 +2002,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>18</v>
       </c>
@@ -2053,7 +2076,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H18" t="s">
         <v>26</v>
       </c>
@@ -2091,514 +2114,513 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:36" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21" s="3">
-        <v>1</v>
-      </c>
-      <c r="C21" s="3">
-        <v>2</v>
-      </c>
-      <c r="D21" s="3">
-        <v>3</v>
-      </c>
-      <c r="E21" s="3">
-        <v>4</v>
-      </c>
-      <c r="F21" s="3">
-        <v>5</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I21" s="3">
+    <row r="21" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P21" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="W21" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD21" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="AL21" s="14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="3">
+        <v>1</v>
+      </c>
+      <c r="C22" s="3">
+        <v>2</v>
+      </c>
+      <c r="D22" s="3">
+        <v>3</v>
+      </c>
+      <c r="E22" s="3">
+        <v>4</v>
+      </c>
+      <c r="F22" s="3">
+        <v>5</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I22" s="3">
         <v>6</v>
       </c>
-      <c r="J21" s="3">
+      <c r="J22" s="3">
         <v>7</v>
       </c>
-      <c r="K21" s="3">
+      <c r="K22" s="3">
         <v>8</v>
       </c>
-      <c r="L21" s="3">
+      <c r="L22" s="3">
         <v>9</v>
       </c>
-      <c r="M21" s="3">
+      <c r="M22" s="3">
         <v>10</v>
       </c>
-      <c r="N21" s="11">
+      <c r="N22" s="11">
         <v>11</v>
       </c>
-      <c r="P21" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q21" s="18">
+      <c r="P22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q22" s="18">
         <v>13</v>
       </c>
-      <c r="R21" s="18">
+      <c r="R22" s="18">
         <v>14</v>
       </c>
-      <c r="S21" s="18">
+      <c r="S22" s="18">
         <v>15</v>
       </c>
-      <c r="T21" s="18">
+      <c r="T22" s="18">
         <v>16</v>
       </c>
-      <c r="W21" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="X21" s="3">
+      <c r="W22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="X22" s="3">
         <v>17</v>
       </c>
-      <c r="Y21" s="3">
+      <c r="Y22" s="3">
+        <v>26</v>
+      </c>
+      <c r="Z22" s="3">
+        <v>19</v>
+      </c>
+      <c r="AA22" s="3">
+        <v>20</v>
+      </c>
+      <c r="AB22" s="3">
+        <v>21</v>
+      </c>
+      <c r="AD22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE22" s="3">
+        <v>22</v>
+      </c>
+      <c r="AF22" s="3">
+        <v>23</v>
+      </c>
+      <c r="AG22" s="3">
+        <v>24</v>
+      </c>
+      <c r="AH22" s="3">
         <v>18</v>
       </c>
-      <c r="Z21" s="3">
-        <v>19</v>
-      </c>
-      <c r="AA21" s="3">
-        <v>20</v>
-      </c>
-      <c r="AB21" s="3">
-        <v>21</v>
-      </c>
-      <c r="AD21" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="AE21" s="3">
-        <v>22</v>
-      </c>
-      <c r="AF21" s="3">
-        <v>23</v>
-      </c>
-      <c r="AG21" s="3">
-        <v>24</v>
-      </c>
-      <c r="AH21" s="3">
-        <v>25</v>
-      </c>
-      <c r="AI21" s="3">
-        <v>26</v>
-      </c>
-      <c r="AJ21" s="3">
+      <c r="AI22" s="3">
         <v>29</v>
       </c>
-    </row>
-    <row r="22" spans="1:36" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="15">
-        <v>1</v>
-      </c>
-      <c r="B22" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="26"/>
-      <c r="H22" s="15">
+      <c r="AJ22" s="3"/>
+      <c r="AL22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AM22" s="3">
+        <v>30</v>
+      </c>
+      <c r="AN22" s="3">
+        <v>31</v>
+      </c>
+      <c r="AO22" s="3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A23" s="15">
+        <v>1</v>
+      </c>
+      <c r="B23" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="26"/>
+      <c r="H23" s="15">
         <v>6</v>
       </c>
-      <c r="I22" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="6"/>
-      <c r="N22" s="8"/>
-      <c r="P22" s="20">
-        <v>10</v>
-      </c>
-      <c r="Q22" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="R22" s="19"/>
-      <c r="S22" s="19"/>
-      <c r="T22" s="19"/>
-      <c r="W22" s="21">
-        <v>25</v>
-      </c>
-      <c r="X22" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y22" s="19"/>
-      <c r="Z22" s="19"/>
-      <c r="AA22" s="19"/>
-      <c r="AB22" s="19"/>
-      <c r="AD22" s="21">
-        <v>22</v>
-      </c>
-      <c r="AE22" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="AF22" s="19"/>
-      <c r="AG22" s="19"/>
-      <c r="AH22" s="19"/>
-      <c r="AI22" s="19"/>
-      <c r="AJ22" s="23"/>
-    </row>
-    <row r="23" spans="1:36" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="16">
-        <v>2</v>
-      </c>
-      <c r="B23" s="27"/>
-      <c r="C23" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="28"/>
-      <c r="H23" s="16">
-        <v>7</v>
-      </c>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="8"/>
+      <c r="I23" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="6"/>
       <c r="N23" s="8"/>
       <c r="P23" s="20">
-        <v>14</v>
-      </c>
-      <c r="Q23" s="19"/>
-      <c r="R23" s="19" t="s">
-        <v>2</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="Q23" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="R23" s="19"/>
       <c r="S23" s="19"/>
       <c r="T23" s="19"/>
       <c r="W23" s="21">
-        <v>18</v>
-      </c>
-      <c r="X23" s="19"/>
-      <c r="Y23" s="19" t="s">
-        <v>2</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="X23" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y23" s="19"/>
       <c r="Z23" s="19"/>
       <c r="AA23" s="19"/>
       <c r="AB23" s="19"/>
       <c r="AD23" s="21">
-        <v>23</v>
-      </c>
-      <c r="AE23" s="19"/>
-      <c r="AF23" s="19" t="s">
-        <v>2</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="AE23" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF23" s="19"/>
       <c r="AG23" s="19"/>
       <c r="AH23" s="19"/>
       <c r="AI23" s="19"/>
-      <c r="AJ23" s="23"/>
-    </row>
-    <row r="24" spans="1:36" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AJ23" s="33"/>
+      <c r="AL23" s="21">
+        <v>25</v>
+      </c>
+      <c r="AM23" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="AN23" s="19"/>
+      <c r="AO23" s="19"/>
+      <c r="AP23" s="32"/>
+    </row>
+    <row r="24" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27" t="s">
-        <v>2</v>
-      </c>
+      <c r="C24" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="27"/>
       <c r="E24" s="27"/>
       <c r="F24" s="28"/>
       <c r="H24" s="16">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="J24" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="K24" s="7"/>
       <c r="L24" s="7"/>
       <c r="M24" s="8"/>
       <c r="N24" s="8"/>
       <c r="P24" s="20">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q24" s="19"/>
-      <c r="R24" s="19"/>
-      <c r="S24" s="19" t="s">
-        <v>2</v>
-      </c>
+      <c r="R24" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="S24" s="19"/>
       <c r="T24" s="19"/>
       <c r="W24" s="21">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="X24" s="19"/>
-      <c r="Y24" s="19"/>
-      <c r="Z24" s="19" t="s">
-        <v>2</v>
-      </c>
+      <c r="Y24" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z24" s="19"/>
       <c r="AA24" s="19"/>
       <c r="AB24" s="19"/>
       <c r="AD24" s="21">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AE24" s="19"/>
-      <c r="AF24" s="19"/>
-      <c r="AG24" s="19" t="s">
-        <v>2</v>
-      </c>
+      <c r="AF24" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG24" s="19"/>
       <c r="AH24" s="19"/>
       <c r="AI24" s="19"/>
-      <c r="AJ24" s="23"/>
-    </row>
-    <row r="25" spans="1:36" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AJ24" s="33"/>
+      <c r="AL24" s="21">
+        <v>30</v>
+      </c>
+      <c r="AM24" s="19"/>
+      <c r="AN24" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="AO24" s="19"/>
+      <c r="AP24" s="32"/>
+    </row>
+    <row r="25" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B25" s="27"/>
       <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27" t="s">
-        <v>2</v>
-      </c>
+      <c r="D25" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" s="27"/>
       <c r="F25" s="28"/>
       <c r="H25" s="16">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="K25" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L25" s="7"/>
       <c r="M25" s="8"/>
       <c r="N25" s="8"/>
       <c r="P25" s="20">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Q25" s="19"/>
       <c r="R25" s="19"/>
-      <c r="S25" s="19"/>
-      <c r="T25" s="19" t="s">
-        <v>2</v>
-      </c>
+      <c r="S25" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="T25" s="19"/>
       <c r="W25" s="21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="X25" s="19"/>
       <c r="Y25" s="19"/>
-      <c r="Z25" s="19"/>
-      <c r="AA25" s="19" t="s">
-        <v>2</v>
-      </c>
+      <c r="Z25" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA25" s="19"/>
       <c r="AB25" s="19"/>
       <c r="AD25" s="21">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="AE25" s="19"/>
       <c r="AF25" s="19"/>
-      <c r="AG25" s="19"/>
-      <c r="AH25" s="19" t="s">
-        <v>2</v>
-      </c>
+      <c r="AG25" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH25" s="19"/>
       <c r="AI25" s="19"/>
-      <c r="AJ25" s="23"/>
-    </row>
-    <row r="26" spans="1:36" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A26" s="17">
-        <v>5</v>
-      </c>
-      <c r="B26" s="29"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="30" t="s">
-        <v>2</v>
-      </c>
+      <c r="AJ25" s="33"/>
+      <c r="AL25" s="21">
+        <v>31</v>
+      </c>
+      <c r="AM25" s="31"/>
+      <c r="AN25" s="31"/>
+      <c r="AO25" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="AP25" s="32"/>
+    </row>
+    <row r="26" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A26" s="16">
+        <v>4</v>
+      </c>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="F26" s="28"/>
       <c r="H26" s="16">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="I26" s="7"/>
       <c r="J26" s="7"/>
       <c r="K26" s="7"/>
-      <c r="L26" s="7"/>
-      <c r="M26" s="8" t="s">
-        <v>2</v>
-      </c>
+      <c r="L26" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M26" s="8"/>
       <c r="N26" s="8"/>
+      <c r="P26" s="20">
+        <v>16</v>
+      </c>
+      <c r="Q26" s="19"/>
+      <c r="R26" s="19"/>
+      <c r="S26" s="19"/>
+      <c r="T26" s="19" t="s">
+        <v>2</v>
+      </c>
       <c r="W26" s="21">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="X26" s="19"/>
       <c r="Y26" s="19"/>
       <c r="Z26" s="19"/>
-      <c r="AA26" s="19"/>
-      <c r="AB26" s="19" t="s">
-        <v>2</v>
-      </c>
+      <c r="AA26" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB26" s="19"/>
       <c r="AD26" s="21">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="AE26" s="19"/>
       <c r="AF26" s="19"/>
       <c r="AG26" s="19"/>
-      <c r="AH26" s="19"/>
-      <c r="AI26" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="AJ26" s="23"/>
-    </row>
-    <row r="27" spans="1:36" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="H27" s="17">
+      <c r="AH26" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI26" s="19"/>
+      <c r="AJ26" s="33"/>
+      <c r="AL26" s="21">
+        <v>32</v>
+      </c>
+      <c r="AM26" s="32"/>
+      <c r="AN26" s="32"/>
+      <c r="AO26" s="32"/>
+      <c r="AP26" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A27" s="17">
+        <v>5</v>
+      </c>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="H27" s="16">
+        <v>13</v>
+      </c>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="N27" s="8"/>
+      <c r="W27" s="21">
+        <v>21</v>
+      </c>
+      <c r="X27" s="19"/>
+      <c r="Y27" s="19"/>
+      <c r="Z27" s="19"/>
+      <c r="AA27" s="19"/>
+      <c r="AB27" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD27" s="21">
+        <v>29</v>
+      </c>
+      <c r="AE27" s="19"/>
+      <c r="AF27" s="19"/>
+      <c r="AG27" s="19"/>
+      <c r="AH27" s="19"/>
+      <c r="AI27" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ27" s="33"/>
+    </row>
+    <row r="28" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="H28" s="17">
         <v>11</v>
       </c>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
-      <c r="L27" s="9"/>
-      <c r="M27" s="10"/>
-      <c r="N27" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD27" s="20">
-        <v>29</v>
-      </c>
-      <c r="AE27" s="23"/>
-      <c r="AF27" s="23"/>
-      <c r="AG27" s="23"/>
-      <c r="AH27" s="23"/>
-      <c r="AI27" s="23"/>
-      <c r="AJ27" s="23" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD28" s="34"/>
+      <c r="AE28" s="25"/>
+      <c r="AF28" s="25"/>
+      <c r="AG28" s="25"/>
+      <c r="AH28" s="25"/>
+      <c r="AI28" s="25"/>
+      <c r="AJ28" s="27"/>
+    </row>
+    <row r="31" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="H31" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B31" s="2" t="s">
+    <row r="32" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B32" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="E32" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F32" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I31" s="2" t="s">
+      <c r="I32" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J31" s="2" t="s">
+      <c r="J32" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K31" s="2" t="s">
+      <c r="K32" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L31" s="2" t="s">
+      <c r="L32" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M31" s="2" t="s">
+      <c r="M32" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="P31" s="2" t="s">
+      <c r="P32" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="W31" s="2" t="s">
+      <c r="W32" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="X31" s="2"/>
-      <c r="Y31" s="2"/>
-      <c r="Z31" s="2"/>
-      <c r="AA31" s="2"/>
-      <c r="AB31" s="2"/>
-      <c r="AD31" s="2" t="s">
+      <c r="X32" s="2"/>
+      <c r="Y32" s="2"/>
+      <c r="Z32" s="2"/>
+      <c r="AA32" s="2"/>
+      <c r="AB32" s="2"/>
+      <c r="AD32" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="AE31" s="2"/>
-      <c r="AF31" s="2"/>
-      <c r="AG31" s="2"/>
-      <c r="AH31" s="2"/>
-      <c r="AI31" s="2"/>
-    </row>
-    <row r="32" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+      <c r="AE32" s="2"/>
+      <c r="AF32" s="2"/>
+      <c r="AG32" s="2"/>
+      <c r="AH32" s="2"/>
+      <c r="AI32" s="2"/>
+      <c r="AL32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AM32" s="2"/>
+      <c r="AN32" s="2"/>
+      <c r="AO32" s="2"/>
+      <c r="AP32" s="2"/>
+      <c r="AQ32" s="2"/>
+    </row>
+    <row r="33" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="B32" s="2">
-        <v>4</v>
-      </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="H32" t="s">
-        <v>21</v>
-      </c>
-      <c r="I32" s="2">
-        <v>5</v>
-      </c>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-      <c r="P32" s="13"/>
-      <c r="Q32" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="R32" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="S32" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="T32" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="U32" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="V32" s="2"/>
-      <c r="W32" s="2"/>
-      <c r="X32" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y32" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="Z32" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="AA32" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB32" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="AD32" s="2"/>
-      <c r="AE32" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AF32" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="AG32" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="AH32" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="AI32" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="B33" s="2">
         <v>4</v>
@@ -2608,7 +2630,7 @@
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="H33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I33" s="2">
         <v>5</v>
@@ -2617,41 +2639,75 @@
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
       <c r="M33" s="4"/>
-      <c r="P33" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q33" s="2">
-        <v>3</v>
-      </c>
-      <c r="R33" s="2"/>
-      <c r="S33" s="2"/>
-      <c r="T33" s="2"/>
-      <c r="U33" s="2"/>
+      <c r="P33" s="13"/>
+      <c r="Q33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="R33" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="S33" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="U33" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="V33" s="2"/>
-      <c r="W33" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="X33" s="2">
-        <v>4</v>
-      </c>
-      <c r="Y33" s="2"/>
-      <c r="Z33" s="2"/>
-      <c r="AA33" s="2"/>
-      <c r="AB33" s="2"/>
-      <c r="AD33" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AE33" s="2">
-        <v>5</v>
-      </c>
-      <c r="AF33" s="2"/>
-      <c r="AG33" s="2"/>
-      <c r="AH33" s="2"/>
-      <c r="AI33" s="2"/>
-    </row>
-    <row r="34" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="W33" s="2"/>
+      <c r="X33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y33" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z33" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD33" s="2"/>
+      <c r="AE33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF33" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG33" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AI33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL33" s="2"/>
+      <c r="AM33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AN33" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AO33" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AP33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AQ33" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B34" s="2">
         <v>4</v>
@@ -2661,7 +2717,7 @@
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="H34" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I34" s="2">
         <v>5</v>
@@ -2670,8 +2726,8 @@
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
-      <c r="P34" s="13" t="s">
-        <v>33</v>
+      <c r="P34" t="s">
+        <v>25</v>
       </c>
       <c r="Q34" s="2">
         <v>3</v>
@@ -2682,7 +2738,7 @@
       <c r="U34" s="2"/>
       <c r="V34" s="2"/>
       <c r="W34" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="X34" s="2">
         <v>4</v>
@@ -2692,7 +2748,7 @@
       <c r="AA34" s="2"/>
       <c r="AB34" s="2"/>
       <c r="AD34" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AE34" s="2">
         <v>5</v>
@@ -2701,10 +2757,20 @@
       <c r="AG34" s="2"/>
       <c r="AH34" s="2"/>
       <c r="AI34" s="2"/>
-    </row>
-    <row r="35" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AL34" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AM34" s="2">
+        <v>3</v>
+      </c>
+      <c r="AN34" s="2"/>
+      <c r="AO34" s="2"/>
+      <c r="AP34" s="2"/>
+      <c r="AQ34" s="2"/>
+    </row>
+    <row r="35" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B35" s="2">
         <v>4</v>
@@ -2714,7 +2780,7 @@
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="H35" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I35" s="2">
         <v>5</v>
@@ -2724,7 +2790,7 @@
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
       <c r="P35" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q35" s="2">
         <v>3</v>
@@ -2735,7 +2801,7 @@
       <c r="U35" s="2"/>
       <c r="V35" s="2"/>
       <c r="W35" s="2" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="X35" s="2">
         <v>4</v>
@@ -2745,7 +2811,7 @@
       <c r="AA35" s="2"/>
       <c r="AB35" s="2"/>
       <c r="AD35" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AE35" s="2">
         <v>5</v>
@@ -2754,10 +2820,20 @@
       <c r="AG35" s="2"/>
       <c r="AH35" s="2"/>
       <c r="AI35" s="2"/>
-    </row>
-    <row r="36" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AL35" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM35" s="2">
+        <v>3</v>
+      </c>
+      <c r="AN35" s="2"/>
+      <c r="AO35" s="2"/>
+      <c r="AP35" s="2"/>
+      <c r="AQ35" s="2"/>
+    </row>
+    <row r="36" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B36" s="2">
         <v>4</v>
@@ -2767,7 +2843,7 @@
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="H36" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="I36" s="2">
         <v>5</v>
@@ -2777,7 +2853,7 @@
       <c r="L36" s="4"/>
       <c r="M36" s="4"/>
       <c r="P36" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q36" s="2">
         <v>3</v>
@@ -2788,7 +2864,7 @@
       <c r="U36" s="2"/>
       <c r="V36" s="2"/>
       <c r="W36" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="X36" s="2">
         <v>4</v>
@@ -2798,7 +2874,7 @@
       <c r="AA36" s="2"/>
       <c r="AB36" s="2"/>
       <c r="AD36" s="2" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="AE36" s="2">
         <v>5</v>
@@ -2807,10 +2883,30 @@
       <c r="AG36" s="2"/>
       <c r="AH36" s="2"/>
       <c r="AI36" s="2"/>
-    </row>
-    <row r="37" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AL36" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM36" s="2">
+        <v>3</v>
+      </c>
+      <c r="AN36" s="2"/>
+      <c r="AO36" s="2"/>
+      <c r="AP36" s="2"/>
+      <c r="AQ36" s="2"/>
+    </row>
+    <row r="37" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37" s="2">
+        <v>4</v>
+      </c>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
       <c r="H37" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="I37" s="2">
         <v>5</v>
@@ -2819,8 +2915,19 @@
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
+      <c r="P37" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q37" s="2">
+        <v>3</v>
+      </c>
+      <c r="R37" s="2"/>
+      <c r="S37" s="2"/>
+      <c r="T37" s="2"/>
+      <c r="U37" s="2"/>
+      <c r="V37" s="2"/>
       <c r="W37" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="X37" s="2">
         <v>4</v>
@@ -2830,7 +2937,7 @@
       <c r="AA37" s="2"/>
       <c r="AB37" s="2"/>
       <c r="AD37" s="2" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="AE37" s="2">
         <v>5</v>
@@ -2839,8 +2946,34 @@
       <c r="AG37" s="2"/>
       <c r="AH37" s="2"/>
       <c r="AI37" s="2"/>
-    </row>
-    <row r="38" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AL37" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AM37" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H38" t="s">
+        <v>26</v>
+      </c>
+      <c r="I38" s="2">
+        <v>5</v>
+      </c>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="4"/>
+      <c r="M38" s="4"/>
+      <c r="W38" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="X38" s="2">
+        <v>4</v>
+      </c>
+      <c r="Y38" s="2"/>
+      <c r="Z38" s="2"/>
+      <c r="AA38" s="2"/>
+      <c r="AB38" s="2"/>
       <c r="AD38" s="2" t="s">
         <v>53</v>
       </c>
@@ -2851,6 +2984,13 @@
       <c r="AG38" s="2"/>
       <c r="AH38" s="2"/>
       <c r="AI38" s="2"/>
+    </row>
+    <row r="39" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AE39" s="2"/>
+      <c r="AF39" s="2"/>
+      <c r="AG39" s="2"/>
+      <c r="AH39" s="2"/>
+      <c r="AI39" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Small improvement to email-sending process, more entry of test data and added check for 3-3 scores in results-entry
</commit_message>
<xml_diff>
--- a/test-data.xlsx
+++ b/test-data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="74">
   <si>
     <t>Division 1</t>
   </si>
@@ -129,9 +129,6 @@
     <t>Berneice Zebrowski</t>
   </si>
   <si>
-    <t>Libby Green</t>
-  </si>
-  <si>
     <t>Dann Emberton</t>
   </si>
   <si>
@@ -211,6 +208,45 @@
   </si>
   <si>
     <t>Sherika Obermillery</t>
+  </si>
+  <si>
+    <t>Wed 15</t>
+  </si>
+  <si>
+    <t>Thu 23</t>
+  </si>
+  <si>
+    <t>Mon 13</t>
+  </si>
+  <si>
+    <t>Thu 16</t>
+  </si>
+  <si>
+    <t>Tue 28</t>
+  </si>
+  <si>
+    <t>Sat 18</t>
+  </si>
+  <si>
+    <t>Fri 24</t>
+  </si>
+  <si>
+    <t>Tue 21</t>
+  </si>
+  <si>
+    <t>Sat 25</t>
+  </si>
+  <si>
+    <t>Mon 20</t>
+  </si>
+  <si>
+    <t>Wed 22</t>
+  </si>
+  <si>
+    <t>Fri 17</t>
+  </si>
+  <si>
+    <t>Fri 31</t>
   </si>
 </sst>
 </file>
@@ -376,7 +412,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -465,7 +501,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -754,8 +789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X11" workbookViewId="0">
-      <selection activeCell="AF25" sqref="AF25"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="M35" sqref="M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,13 +814,13 @@
         <v>31</v>
       </c>
       <c r="W1" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AD1" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AL1" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
@@ -1633,7 +1668,7 @@
       </c>
       <c r="V13" s="2"/>
       <c r="W13" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X13" s="2">
         <v>4</v>
@@ -1651,7 +1686,7 @@
         <v>16</v>
       </c>
       <c r="AD13" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AE13" s="2">
         <v>5</v>
@@ -1669,7 +1704,7 @@
         <v>13</v>
       </c>
       <c r="AL13" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AM13" s="2">
         <v>2</v>
@@ -1744,7 +1779,7 @@
       </c>
       <c r="V14" s="2"/>
       <c r="W14" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="X14" s="2">
         <v>4</v>
@@ -1762,7 +1797,7 @@
         <v>6</v>
       </c>
       <c r="AD14" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AE14" s="2">
         <v>5</v>
@@ -1780,7 +1815,7 @@
         <v>13</v>
       </c>
       <c r="AL14" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AM14" s="2">
         <v>2</v>
@@ -1836,7 +1871,7 @@
         <v>10</v>
       </c>
       <c r="P15" s="13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="Q15" s="2">
         <v>3</v>
@@ -1855,7 +1890,7 @@
       </c>
       <c r="V15" s="2"/>
       <c r="W15" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="X15" s="2">
         <v>4</v>
@@ -1873,7 +1908,7 @@
         <v>13</v>
       </c>
       <c r="AD15" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AE15" s="2">
         <v>5</v>
@@ -1891,7 +1926,7 @@
         <v>13</v>
       </c>
       <c r="AL15" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AM15" s="2">
         <v>2</v>
@@ -1947,7 +1982,7 @@
         <v>24</v>
       </c>
       <c r="P16" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q16" s="2">
         <v>3</v>
@@ -1966,7 +2001,7 @@
       </c>
       <c r="V16" s="2"/>
       <c r="W16" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="X16" s="2">
         <v>4</v>
@@ -1984,7 +2019,7 @@
         <v>14</v>
       </c>
       <c r="AD16" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AE16" s="2">
         <v>5</v>
@@ -2040,7 +2075,7 @@
         <v>11</v>
       </c>
       <c r="W17" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="X17" s="2">
         <v>4</v>
@@ -2058,7 +2093,7 @@
         <v>11</v>
       </c>
       <c r="AD17" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AE17" s="2">
         <v>5</v>
@@ -2096,7 +2131,7 @@
         <v>16</v>
       </c>
       <c r="AD18" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AE18" s="2">
         <v>5</v>
@@ -2125,13 +2160,13 @@
         <v>31</v>
       </c>
       <c r="W21" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AD21" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AL21" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
@@ -2169,7 +2204,7 @@
         <v>9</v>
       </c>
       <c r="M22" s="3">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="N22" s="11">
         <v>11</v>
@@ -2178,7 +2213,7 @@
         <v>3</v>
       </c>
       <c r="Q22" s="18">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="R22" s="18">
         <v>14</v>
@@ -2230,12 +2265,15 @@
         <v>3</v>
       </c>
       <c r="AM22" s="3">
+        <v>25</v>
+      </c>
+      <c r="AN22" s="3">
         <v>30</v>
       </c>
-      <c r="AN22" s="3">
+      <c r="AO22" s="3">
         <v>31</v>
       </c>
-      <c r="AO22" s="3">
+      <c r="AP22" s="3">
         <v>32</v>
       </c>
     </row>
@@ -2246,243 +2284,427 @@
       <c r="B23" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="26"/>
+      <c r="C23" s="25">
+        <v>3</v>
+      </c>
+      <c r="D23" s="25">
+        <v>3</v>
+      </c>
+      <c r="E23" s="25">
+        <v>2</v>
+      </c>
+      <c r="F23" s="26">
+        <v>3</v>
+      </c>
       <c r="H23" s="15">
         <v>6</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="6"/>
-      <c r="N23" s="8"/>
+      <c r="J23" s="5">
+        <v>2</v>
+      </c>
+      <c r="K23" s="5">
+        <v>3</v>
+      </c>
+      <c r="L23" s="5">
+        <v>2</v>
+      </c>
+      <c r="M23" s="6">
+        <v>2</v>
+      </c>
+      <c r="N23" s="8">
+        <v>3</v>
+      </c>
       <c r="P23" s="20">
         <v>10</v>
       </c>
       <c r="Q23" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="R23" s="19"/>
-      <c r="S23" s="19"/>
-      <c r="T23" s="19"/>
+      <c r="R23" s="19">
+        <v>3</v>
+      </c>
+      <c r="S23" s="19">
+        <v>3</v>
+      </c>
+      <c r="T23" s="19">
+        <v>1</v>
+      </c>
       <c r="W23" s="21">
         <v>17</v>
       </c>
       <c r="X23" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="Y23" s="19"/>
-      <c r="Z23" s="19"/>
-      <c r="AA23" s="19"/>
-      <c r="AB23" s="19"/>
+      <c r="Y23" s="19">
+        <v>3</v>
+      </c>
+      <c r="Z23" s="19">
+        <v>2</v>
+      </c>
+      <c r="AA23" s="19">
+        <v>3</v>
+      </c>
+      <c r="AB23" s="19">
+        <v>3</v>
+      </c>
       <c r="AD23" s="21">
         <v>22</v>
       </c>
       <c r="AE23" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="AF23" s="19"/>
-      <c r="AG23" s="19"/>
-      <c r="AH23" s="19"/>
-      <c r="AI23" s="19"/>
-      <c r="AJ23" s="33"/>
+      <c r="AF23" s="19">
+        <v>2</v>
+      </c>
+      <c r="AG23" s="19">
+        <v>3</v>
+      </c>
+      <c r="AH23" s="19">
+        <v>0</v>
+      </c>
+      <c r="AI23" s="19">
+        <v>3</v>
+      </c>
+      <c r="AJ23" s="32"/>
       <c r="AL23" s="21">
         <v>25</v>
       </c>
       <c r="AM23" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="AN23" s="19"/>
-      <c r="AO23" s="19"/>
-      <c r="AP23" s="32"/>
+      <c r="AN23" s="19">
+        <v>3</v>
+      </c>
+      <c r="AO23" s="19">
+        <v>3</v>
+      </c>
+      <c r="AP23" s="19">
+        <v>3</v>
+      </c>
     </row>
     <row r="24" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="16">
         <v>2</v>
       </c>
-      <c r="B24" s="27"/>
+      <c r="B24" s="27">
+        <v>2</v>
+      </c>
       <c r="C24" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="28"/>
+      <c r="D24" s="27">
+        <v>1</v>
+      </c>
+      <c r="E24" s="27">
+        <v>3</v>
+      </c>
+      <c r="F24" s="28">
+        <v>2</v>
+      </c>
       <c r="H24" s="16">
         <v>7</v>
       </c>
-      <c r="I24" s="7"/>
+      <c r="I24" s="7">
+        <v>3</v>
+      </c>
       <c r="J24" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="8"/>
-      <c r="N24" s="8"/>
+      <c r="K24" s="7">
+        <v>3</v>
+      </c>
+      <c r="L24" s="7">
+        <v>3</v>
+      </c>
+      <c r="M24" s="8">
+        <v>1</v>
+      </c>
+      <c r="N24" s="8">
+        <v>2</v>
+      </c>
       <c r="P24" s="20">
         <v>14</v>
       </c>
-      <c r="Q24" s="19"/>
+      <c r="Q24" s="19">
+        <v>1</v>
+      </c>
       <c r="R24" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="S24" s="19"/>
-      <c r="T24" s="19"/>
+      <c r="S24" s="19">
+        <v>2</v>
+      </c>
+      <c r="T24" s="19">
+        <v>3</v>
+      </c>
       <c r="W24" s="21">
         <v>26</v>
       </c>
-      <c r="X24" s="19"/>
+      <c r="X24" s="19">
+        <v>1</v>
+      </c>
       <c r="Y24" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="Z24" s="19"/>
-      <c r="AA24" s="19"/>
-      <c r="AB24" s="19"/>
+      <c r="Z24" s="19">
+        <v>3</v>
+      </c>
+      <c r="AA24" s="19">
+        <v>1</v>
+      </c>
+      <c r="AB24" s="19">
+        <v>0</v>
+      </c>
       <c r="AD24" s="21">
         <v>23</v>
       </c>
-      <c r="AE24" s="19"/>
+      <c r="AE24" s="19">
+        <v>1</v>
+      </c>
       <c r="AF24" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="AG24" s="19"/>
-      <c r="AH24" s="19"/>
-      <c r="AI24" s="19"/>
-      <c r="AJ24" s="33"/>
+      <c r="AG24" s="19">
+        <v>3</v>
+      </c>
+      <c r="AH24" s="19">
+        <v>1</v>
+      </c>
+      <c r="AI24" s="19">
+        <v>2</v>
+      </c>
+      <c r="AJ24" s="32"/>
       <c r="AL24" s="21">
         <v>30</v>
       </c>
-      <c r="AM24" s="19"/>
+      <c r="AM24" s="19">
+        <v>1</v>
+      </c>
       <c r="AN24" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="AO24" s="19"/>
-      <c r="AP24" s="32"/>
+      <c r="AO24" s="19">
+        <v>3</v>
+      </c>
+      <c r="AP24" s="19">
+        <v>2</v>
+      </c>
     </row>
     <row r="25" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="16">
         <v>3</v>
       </c>
-      <c r="B25" s="27"/>
-      <c r="C25" s="27"/>
+      <c r="B25" s="27">
+        <v>0</v>
+      </c>
+      <c r="C25" s="27">
+        <v>3</v>
+      </c>
       <c r="D25" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="E25" s="27"/>
-      <c r="F25" s="28"/>
+      <c r="E25" s="27">
+        <v>3</v>
+      </c>
+      <c r="F25" s="28">
+        <v>1</v>
+      </c>
       <c r="H25" s="16">
         <v>8</v>
       </c>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
+      <c r="I25" s="7">
+        <v>1</v>
+      </c>
+      <c r="J25" s="7">
+        <v>2</v>
+      </c>
       <c r="K25" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="L25" s="7"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="8"/>
+      <c r="L25" s="7">
+        <v>2</v>
+      </c>
+      <c r="M25" s="8">
+        <v>3</v>
+      </c>
+      <c r="N25" s="8">
+        <v>0</v>
+      </c>
       <c r="P25" s="20">
         <v>15</v>
       </c>
-      <c r="Q25" s="19"/>
-      <c r="R25" s="19"/>
+      <c r="Q25" s="19">
+        <v>2</v>
+      </c>
+      <c r="R25" s="19">
+        <v>1</v>
+      </c>
       <c r="S25" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="T25" s="19"/>
+      <c r="T25" s="19">
+        <v>3</v>
+      </c>
       <c r="W25" s="21">
         <v>19</v>
       </c>
-      <c r="X25" s="19"/>
-      <c r="Y25" s="19"/>
+      <c r="X25" s="19">
+        <v>2</v>
+      </c>
+      <c r="Y25" s="19">
+        <v>2</v>
+      </c>
       <c r="Z25" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="AA25" s="19"/>
-      <c r="AB25" s="19"/>
+      <c r="AA25" s="19">
+        <v>3</v>
+      </c>
+      <c r="AB25" s="19">
+        <v>1</v>
+      </c>
       <c r="AD25" s="21">
         <v>24</v>
       </c>
-      <c r="AE25" s="19"/>
-      <c r="AF25" s="19"/>
+      <c r="AE25" s="19">
+        <v>2</v>
+      </c>
+      <c r="AF25" s="19">
+        <v>0</v>
+      </c>
       <c r="AG25" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="AH25" s="19"/>
-      <c r="AI25" s="19"/>
-      <c r="AJ25" s="33"/>
+      <c r="AH25" s="19">
+        <v>2</v>
+      </c>
+      <c r="AI25" s="19">
+        <v>3</v>
+      </c>
+      <c r="AJ25" s="32"/>
       <c r="AL25" s="21">
         <v>31</v>
       </c>
-      <c r="AM25" s="31"/>
-      <c r="AN25" s="31"/>
+      <c r="AM25" s="31">
+        <v>2</v>
+      </c>
+      <c r="AN25" s="31">
+        <v>2</v>
+      </c>
       <c r="AO25" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="AP25" s="32"/>
+      <c r="AP25" s="19">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="16">
         <v>4</v>
       </c>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
+      <c r="B26" s="27">
+        <v>2</v>
+      </c>
+      <c r="C26" s="27">
+        <v>0</v>
+      </c>
+      <c r="D26" s="27">
+        <v>2</v>
+      </c>
       <c r="E26" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="F26" s="28"/>
+      <c r="F26" s="28">
+        <v>2</v>
+      </c>
       <c r="H26" s="16">
         <v>9</v>
       </c>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
+      <c r="I26" s="7">
+        <v>0</v>
+      </c>
+      <c r="J26" s="7">
+        <v>0</v>
+      </c>
+      <c r="K26" s="7">
+        <v>2</v>
+      </c>
       <c r="L26" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="M26" s="8"/>
-      <c r="N26" s="8"/>
+      <c r="M26" s="8">
+        <v>3</v>
+      </c>
+      <c r="N26" s="8">
+        <v>2</v>
+      </c>
       <c r="P26" s="20">
         <v>16</v>
       </c>
-      <c r="Q26" s="19"/>
-      <c r="R26" s="19"/>
-      <c r="S26" s="19"/>
+      <c r="Q26" s="19">
+        <v>3</v>
+      </c>
+      <c r="R26" s="19">
+        <v>0</v>
+      </c>
+      <c r="S26" s="19">
+        <v>2</v>
+      </c>
       <c r="T26" s="19" t="s">
         <v>2</v>
       </c>
       <c r="W26" s="21">
         <v>20</v>
       </c>
-      <c r="X26" s="19"/>
-      <c r="Y26" s="19"/>
-      <c r="Z26" s="19"/>
+      <c r="X26" s="19">
+        <v>0</v>
+      </c>
+      <c r="Y26" s="19">
+        <v>3</v>
+      </c>
+      <c r="Z26" s="19">
+        <v>0</v>
+      </c>
       <c r="AA26" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="AB26" s="19"/>
+      <c r="AB26" s="19">
+        <v>2</v>
+      </c>
       <c r="AD26" s="21">
         <v>18</v>
       </c>
-      <c r="AE26" s="19"/>
-      <c r="AF26" s="19"/>
-      <c r="AG26" s="19"/>
+      <c r="AE26" s="19">
+        <v>3</v>
+      </c>
+      <c r="AF26" s="19">
+        <v>3</v>
+      </c>
+      <c r="AG26" s="19">
+        <v>2</v>
+      </c>
       <c r="AH26" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="AI26" s="19"/>
-      <c r="AJ26" s="33"/>
+      <c r="AI26" s="19">
+        <v>1</v>
+      </c>
+      <c r="AJ26" s="32"/>
       <c r="AL26" s="21">
         <v>32</v>
       </c>
-      <c r="AM26" s="32"/>
-      <c r="AN26" s="32"/>
-      <c r="AO26" s="32"/>
+      <c r="AM26" s="19">
+        <v>0</v>
+      </c>
+      <c r="AN26" s="19">
+        <v>3</v>
+      </c>
+      <c r="AO26" s="19">
+        <v>2</v>
+      </c>
       <c r="AP26" s="19" t="s">
         <v>2</v>
       </c>
@@ -2491,59 +2713,103 @@
       <c r="A27" s="17">
         <v>5</v>
       </c>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
+      <c r="B27" s="29">
+        <v>1</v>
+      </c>
+      <c r="C27" s="29">
+        <v>1</v>
+      </c>
+      <c r="D27" s="29">
+        <v>3</v>
+      </c>
+      <c r="E27" s="29">
+        <v>2</v>
+      </c>
       <c r="F27" s="30" t="s">
         <v>2</v>
       </c>
       <c r="H27" s="16">
         <v>13</v>
       </c>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="7"/>
+      <c r="I27" s="7">
+        <v>3</v>
+      </c>
+      <c r="J27" s="7">
+        <v>2</v>
+      </c>
+      <c r="K27" s="7">
+        <v>1</v>
+      </c>
+      <c r="L27" s="7">
+        <v>1</v>
+      </c>
       <c r="M27" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="N27" s="8"/>
+      <c r="N27" s="8">
+        <v>2</v>
+      </c>
       <c r="W27" s="21">
         <v>21</v>
       </c>
-      <c r="X27" s="19"/>
-      <c r="Y27" s="19"/>
-      <c r="Z27" s="19"/>
-      <c r="AA27" s="19"/>
+      <c r="X27" s="19">
+        <v>1</v>
+      </c>
+      <c r="Y27" s="19">
+        <v>3</v>
+      </c>
+      <c r="Z27" s="19">
+        <v>2</v>
+      </c>
+      <c r="AA27" s="19">
+        <v>3</v>
+      </c>
       <c r="AB27" s="19" t="s">
         <v>2</v>
       </c>
       <c r="AD27" s="21">
         <v>29</v>
       </c>
-      <c r="AE27" s="19"/>
-      <c r="AF27" s="19"/>
-      <c r="AG27" s="19"/>
-      <c r="AH27" s="19"/>
+      <c r="AE27" s="19">
+        <v>1</v>
+      </c>
+      <c r="AF27" s="19">
+        <v>3</v>
+      </c>
+      <c r="AG27" s="19">
+        <v>1</v>
+      </c>
+      <c r="AH27" s="19">
+        <v>2</v>
+      </c>
       <c r="AI27" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="AJ27" s="33"/>
+      <c r="AJ27" s="32"/>
     </row>
     <row r="28" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
       <c r="H28" s="17">
         <v>11</v>
       </c>
-      <c r="I28" s="9"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="9"/>
-      <c r="M28" s="10"/>
+      <c r="I28" s="9">
+        <v>1</v>
+      </c>
+      <c r="J28" s="9">
+        <v>1</v>
+      </c>
+      <c r="K28" s="9">
+        <v>3</v>
+      </c>
+      <c r="L28" s="9">
+        <v>1</v>
+      </c>
+      <c r="M28" s="10">
+        <v>3</v>
+      </c>
       <c r="N28" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="AD28" s="34"/>
+      <c r="AD28" s="33"/>
       <c r="AE28" s="25"/>
       <c r="AF28" s="25"/>
       <c r="AG28" s="25"/>
@@ -2625,20 +2891,36 @@
       <c r="B33" s="2">
         <v>4</v>
       </c>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
+      <c r="C33" s="2">
+        <v>3</v>
+      </c>
+      <c r="D33" s="2">
+        <v>1</v>
+      </c>
+      <c r="E33" s="2">
+        <v>0</v>
+      </c>
+      <c r="F33" s="2">
+        <v>18</v>
+      </c>
       <c r="H33" t="s">
         <v>21</v>
       </c>
       <c r="I33" s="2">
         <v>5</v>
       </c>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
+      <c r="J33" s="4">
+        <v>3</v>
+      </c>
+      <c r="K33" s="4">
+        <v>0</v>
+      </c>
+      <c r="L33" s="4">
+        <v>2</v>
+      </c>
+      <c r="M33" s="4">
+        <v>19</v>
+      </c>
       <c r="P33" s="13"/>
       <c r="Q33" s="2" t="s">
         <v>6</v>
@@ -2712,61 +2994,109 @@
       <c r="B34" s="2">
         <v>4</v>
       </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
+      <c r="C34" s="2">
+        <v>2</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0</v>
+      </c>
+      <c r="E34" s="2">
+        <v>2</v>
+      </c>
+      <c r="F34" s="2">
+        <v>13</v>
+      </c>
       <c r="H34" t="s">
         <v>22</v>
       </c>
       <c r="I34" s="2">
         <v>5</v>
       </c>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
+      <c r="J34" s="4">
+        <v>4</v>
+      </c>
+      <c r="K34" s="4">
+        <v>0</v>
+      </c>
+      <c r="L34" s="4">
+        <v>1</v>
+      </c>
+      <c r="M34" s="4">
+        <v>20</v>
+      </c>
       <c r="P34" t="s">
         <v>25</v>
       </c>
       <c r="Q34" s="2">
         <v>3</v>
       </c>
-      <c r="R34" s="2"/>
-      <c r="S34" s="2"/>
-      <c r="T34" s="2"/>
-      <c r="U34" s="2"/>
+      <c r="R34" s="2">
+        <v>2</v>
+      </c>
+      <c r="S34" s="2">
+        <v>0</v>
+      </c>
+      <c r="T34" s="2">
+        <v>1</v>
+      </c>
+      <c r="U34" s="2">
+        <v>10</v>
+      </c>
       <c r="V34" s="2"/>
       <c r="W34" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X34" s="2">
         <v>4</v>
       </c>
-      <c r="Y34" s="2"/>
-      <c r="Z34" s="2"/>
-      <c r="AA34" s="2"/>
-      <c r="AB34" s="2"/>
+      <c r="Y34" s="2">
+        <v>3</v>
+      </c>
+      <c r="Z34" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA34" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB34" s="2">
+        <v>19</v>
+      </c>
       <c r="AD34" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AE34" s="2">
-        <v>5</v>
-      </c>
-      <c r="AF34" s="2"/>
-      <c r="AG34" s="2"/>
-      <c r="AH34" s="2"/>
-      <c r="AI34" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="AF34" s="2">
+        <v>3</v>
+      </c>
+      <c r="AG34" s="2">
+        <v>0</v>
+      </c>
+      <c r="AH34" s="2">
+        <v>1</v>
+      </c>
+      <c r="AI34" s="2">
+        <v>13</v>
+      </c>
       <c r="AL34" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AM34" s="2">
         <v>3</v>
       </c>
-      <c r="AN34" s="2"/>
-      <c r="AO34" s="2"/>
-      <c r="AP34" s="2"/>
-      <c r="AQ34" s="2"/>
+      <c r="AN34" s="2">
+        <v>3</v>
+      </c>
+      <c r="AO34" s="2">
+        <v>0</v>
+      </c>
+      <c r="AP34" s="2">
+        <v>0</v>
+      </c>
+      <c r="AQ34" s="2">
+        <v>15</v>
+      </c>
     </row>
     <row r="35" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
@@ -2775,61 +3105,109 @@
       <c r="B35" s="2">
         <v>4</v>
       </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
+      <c r="C35" s="2">
+        <v>2</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0</v>
+      </c>
+      <c r="E35" s="2">
+        <v>2</v>
+      </c>
+      <c r="F35" s="2">
+        <v>10</v>
+      </c>
       <c r="H35" t="s">
         <v>23</v>
       </c>
       <c r="I35" s="2">
         <v>5</v>
       </c>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
+      <c r="J35" s="4">
+        <v>1</v>
+      </c>
+      <c r="K35" s="4">
+        <v>1</v>
+      </c>
+      <c r="L35" s="4">
+        <v>3</v>
+      </c>
+      <c r="M35" s="4">
+        <v>11</v>
+      </c>
       <c r="P35" s="13" t="s">
         <v>33</v>
       </c>
       <c r="Q35" s="2">
         <v>3</v>
       </c>
-      <c r="R35" s="2"/>
-      <c r="S35" s="2"/>
-      <c r="T35" s="2"/>
-      <c r="U35" s="2"/>
+      <c r="R35" s="2">
+        <v>2</v>
+      </c>
+      <c r="S35" s="2">
+        <v>0</v>
+      </c>
+      <c r="T35" s="2">
+        <v>1</v>
+      </c>
+      <c r="U35" s="2">
+        <v>11</v>
+      </c>
       <c r="V35" s="2"/>
       <c r="W35" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="X35" s="2">
         <v>4</v>
       </c>
-      <c r="Y35" s="2"/>
-      <c r="Z35" s="2"/>
-      <c r="AA35" s="2"/>
-      <c r="AB35" s="2"/>
+      <c r="Y35" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z35" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA35" s="2">
+        <v>3</v>
+      </c>
+      <c r="AB35" s="2">
+        <v>6</v>
+      </c>
       <c r="AD35" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AE35" s="2">
-        <v>5</v>
-      </c>
-      <c r="AF35" s="2"/>
-      <c r="AG35" s="2"/>
-      <c r="AH35" s="2"/>
-      <c r="AI35" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="AF35" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG35" s="2">
+        <v>0</v>
+      </c>
+      <c r="AH35" s="2">
+        <v>3</v>
+      </c>
+      <c r="AI35" s="2">
+        <v>11</v>
+      </c>
       <c r="AL35" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AM35" s="2">
         <v>3</v>
       </c>
-      <c r="AN35" s="2"/>
-      <c r="AO35" s="2"/>
-      <c r="AP35" s="2"/>
-      <c r="AQ35" s="2"/>
+      <c r="AN35" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO35" s="2">
+        <v>0</v>
+      </c>
+      <c r="AP35" s="2">
+        <v>2</v>
+      </c>
+      <c r="AQ35" s="2">
+        <v>7</v>
+      </c>
     </row>
     <row r="36" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
@@ -2838,61 +3216,109 @@
       <c r="B36" s="2">
         <v>4</v>
       </c>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
+      <c r="C36" s="2">
+        <v>0</v>
+      </c>
+      <c r="D36" s="2">
+        <v>2</v>
+      </c>
+      <c r="E36" s="2">
+        <v>2</v>
+      </c>
+      <c r="F36" s="2">
+        <v>8</v>
+      </c>
       <c r="H36" t="s">
         <v>24</v>
       </c>
       <c r="I36" s="2">
         <v>5</v>
       </c>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
+      <c r="J36" s="4">
+        <v>2</v>
+      </c>
+      <c r="K36" s="4">
+        <v>1</v>
+      </c>
+      <c r="L36" s="4">
+        <v>2</v>
+      </c>
+      <c r="M36" s="4">
+        <v>13</v>
+      </c>
       <c r="P36" s="13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="Q36" s="2">
         <v>3</v>
       </c>
-      <c r="R36" s="2"/>
-      <c r="S36" s="2"/>
-      <c r="T36" s="2"/>
-      <c r="U36" s="2"/>
+      <c r="R36" s="2">
+        <v>1</v>
+      </c>
+      <c r="S36" s="2">
+        <v>0</v>
+      </c>
+      <c r="T36" s="2">
+        <v>2</v>
+      </c>
+      <c r="U36" s="2">
+        <v>8</v>
+      </c>
       <c r="V36" s="2"/>
       <c r="W36" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="X36" s="2">
         <v>4</v>
       </c>
-      <c r="Y36" s="2"/>
-      <c r="Z36" s="2"/>
-      <c r="AA36" s="2"/>
-      <c r="AB36" s="2"/>
+      <c r="Y36" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z36" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA36" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB36" s="2">
+        <v>13</v>
+      </c>
       <c r="AD36" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AE36" s="2">
-        <v>5</v>
-      </c>
-      <c r="AF36" s="2"/>
-      <c r="AG36" s="2"/>
-      <c r="AH36" s="2"/>
-      <c r="AI36" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="AF36" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG36" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH36" s="2">
+        <v>2</v>
+      </c>
+      <c r="AI36" s="2">
+        <v>10</v>
+      </c>
       <c r="AL36" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AM36" s="2">
         <v>3</v>
       </c>
-      <c r="AN36" s="2"/>
-      <c r="AO36" s="2"/>
-      <c r="AP36" s="2"/>
-      <c r="AQ36" s="2"/>
+      <c r="AN36" s="2">
+        <v>0</v>
+      </c>
+      <c r="AO36" s="2">
+        <v>0</v>
+      </c>
+      <c r="AP36" s="2">
+        <v>3</v>
+      </c>
+      <c r="AQ36" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row r="37" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
@@ -2901,56 +3327,108 @@
       <c r="B37" s="2">
         <v>4</v>
       </c>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
+      <c r="C37" s="2">
+        <v>1</v>
+      </c>
+      <c r="D37" s="2">
+        <v>1</v>
+      </c>
+      <c r="E37" s="2">
+        <v>2</v>
+      </c>
+      <c r="F37" s="2">
+        <v>11</v>
+      </c>
       <c r="H37" t="s">
         <v>32</v>
       </c>
       <c r="I37" s="2">
         <v>5</v>
       </c>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
-      <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
+      <c r="J37" s="4">
+        <v>2</v>
+      </c>
+      <c r="K37" s="4">
+        <v>0</v>
+      </c>
+      <c r="L37" s="4">
+        <v>3</v>
+      </c>
+      <c r="M37" s="4">
+        <v>12</v>
+      </c>
       <c r="P37" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q37" s="2">
         <v>3</v>
       </c>
-      <c r="R37" s="2"/>
-      <c r="S37" s="2"/>
-      <c r="T37" s="2"/>
-      <c r="U37" s="2"/>
+      <c r="R37" s="2">
+        <v>1</v>
+      </c>
+      <c r="S37" s="2">
+        <v>0</v>
+      </c>
+      <c r="T37" s="2">
+        <v>2</v>
+      </c>
+      <c r="U37" s="2">
+        <v>7</v>
+      </c>
       <c r="V37" s="2"/>
       <c r="W37" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="X37" s="2">
         <v>4</v>
       </c>
-      <c r="Y37" s="2"/>
-      <c r="Z37" s="2"/>
-      <c r="AA37" s="2"/>
-      <c r="AB37" s="2"/>
+      <c r="Y37" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z37" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA37" s="2">
+        <v>3</v>
+      </c>
+      <c r="AB37" s="2">
+        <v>7</v>
+      </c>
       <c r="AD37" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AE37" s="2">
-        <v>5</v>
-      </c>
-      <c r="AF37" s="2"/>
-      <c r="AG37" s="2"/>
-      <c r="AH37" s="2"/>
-      <c r="AI37" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="AF37" s="2">
+        <v>2</v>
+      </c>
+      <c r="AG37" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH37" s="2">
+        <v>1</v>
+      </c>
+      <c r="AI37" s="2">
+        <v>16</v>
+      </c>
       <c r="AL37" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AM37" s="2">
         <v>3</v>
+      </c>
+      <c r="AN37" s="2">
+        <v>2</v>
+      </c>
+      <c r="AO37" s="2">
+        <v>0</v>
+      </c>
+      <c r="AP37" s="2">
+        <v>1</v>
+      </c>
+      <c r="AQ37" s="2">
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
@@ -2960,30 +3438,54 @@
       <c r="I38" s="2">
         <v>5</v>
       </c>
-      <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
-      <c r="L38" s="4"/>
-      <c r="M38" s="4"/>
+      <c r="J38" s="4">
+        <v>2</v>
+      </c>
+      <c r="K38" s="4">
+        <v>0</v>
+      </c>
+      <c r="L38" s="4">
+        <v>3</v>
+      </c>
+      <c r="M38" s="4">
+        <v>15</v>
+      </c>
       <c r="W38" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="X38" s="2">
         <v>4</v>
       </c>
-      <c r="Y38" s="2"/>
-      <c r="Z38" s="2"/>
-      <c r="AA38" s="2"/>
-      <c r="AB38" s="2"/>
+      <c r="Y38" s="2">
+        <v>3</v>
+      </c>
+      <c r="Z38" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA38" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB38" s="2">
+        <v>15</v>
+      </c>
       <c r="AD38" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AE38" s="2">
-        <v>5</v>
-      </c>
-      <c r="AF38" s="2"/>
-      <c r="AG38" s="2"/>
-      <c r="AH38" s="2"/>
-      <c r="AI38" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="AF38" s="2">
+        <v>2</v>
+      </c>
+      <c r="AG38" s="2">
+        <v>0</v>
+      </c>
+      <c r="AH38" s="2">
+        <v>2</v>
+      </c>
+      <c r="AI38" s="2">
+        <v>10</v>
+      </c>
     </row>
     <row r="39" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="AE39" s="2"/>
@@ -3000,10 +3502,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3011,11 +3513,13 @@
     <col min="2" max="2" width="18.42578125" style="24" customWidth="1"/>
     <col min="7" max="7" width="10.28515625" customWidth="1"/>
     <col min="8" max="8" width="13.42578125" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" style="24" customWidth="1"/>
+    <col min="17" max="17" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1" s="24" t="s">
         <v>5</v>
@@ -3038,8 +3542,32 @@
       <c r="H1" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3061,11 +3589,35 @@
       <c r="G2" s="4">
         <v>75</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="4">
+        <v>8</v>
+      </c>
+      <c r="M2" s="4">
+        <v>6</v>
+      </c>
+      <c r="N2" s="4">
+        <v>1</v>
+      </c>
+      <c r="O2" s="4">
+        <v>1</v>
+      </c>
+      <c r="P2" s="4">
+        <v>75</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3087,11 +3639,35 @@
       <c r="G3" s="4">
         <v>75</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" s="4">
+        <v>8</v>
+      </c>
+      <c r="M3" s="4">
+        <v>5</v>
+      </c>
+      <c r="N3" s="4">
+        <v>1</v>
+      </c>
+      <c r="O3" s="4">
+        <v>2</v>
+      </c>
+      <c r="P3" s="4">
+        <v>62.5</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3113,11 +3689,35 @@
       <c r="G4" s="4">
         <v>25</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <v>3</v>
+      </c>
+      <c r="K4" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="4">
+        <v>8</v>
+      </c>
+      <c r="M4" s="4">
+        <v>3</v>
+      </c>
+      <c r="N4" s="4">
+        <v>0</v>
+      </c>
+      <c r="O4" s="4">
+        <v>5</v>
+      </c>
+      <c r="P4" s="4">
+        <v>37.5</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3139,11 +3739,35 @@
       <c r="G5" s="4">
         <v>25</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <v>4</v>
+      </c>
+      <c r="K5" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" s="4">
+        <v>8</v>
+      </c>
+      <c r="M5" s="4">
+        <v>1</v>
+      </c>
+      <c r="N5" s="4">
+        <v>2</v>
+      </c>
+      <c r="O5" s="4">
+        <v>5</v>
+      </c>
+      <c r="P5" s="4">
+        <v>12.5</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3165,11 +3789,35 @@
       <c r="G6" s="4">
         <v>25</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <v>5</v>
+      </c>
+      <c r="K6" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" s="4">
+        <v>8</v>
+      </c>
+      <c r="M6" s="4">
+        <v>2</v>
+      </c>
+      <c r="N6" s="4">
+        <v>2</v>
+      </c>
+      <c r="O6" s="4">
+        <v>4</v>
+      </c>
+      <c r="P6" s="4">
+        <v>25</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3191,11 +3839,35 @@
       <c r="G7" s="4">
         <v>40</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <v>6</v>
+      </c>
+      <c r="K7" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" s="4">
+        <v>10</v>
+      </c>
+      <c r="M7" s="4">
+        <v>5</v>
+      </c>
+      <c r="N7" s="4">
+        <v>1</v>
+      </c>
+      <c r="O7" s="4">
+        <v>4</v>
+      </c>
+      <c r="P7" s="4">
+        <v>50</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3217,11 +3889,35 @@
       <c r="G8" s="4">
         <v>20</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <v>7</v>
+      </c>
+      <c r="K8" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="L8" s="4">
+        <v>10</v>
+      </c>
+      <c r="M8" s="4">
+        <v>5</v>
+      </c>
+      <c r="N8" s="4">
+        <v>2</v>
+      </c>
+      <c r="O8" s="4">
+        <v>3</v>
+      </c>
+      <c r="P8" s="4">
+        <v>50</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3243,11 +3939,35 @@
       <c r="G9" s="4">
         <v>20</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <v>8</v>
+      </c>
+      <c r="K9" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="L9" s="4">
+        <v>10</v>
+      </c>
+      <c r="M9" s="4">
+        <v>2</v>
+      </c>
+      <c r="N9" s="4">
+        <v>2</v>
+      </c>
+      <c r="O9" s="4">
+        <v>6</v>
+      </c>
+      <c r="P9" s="4">
+        <v>20</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3269,11 +3989,35 @@
       <c r="G10" s="4">
         <v>100</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <v>9</v>
+      </c>
+      <c r="K10" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="L10" s="4">
+        <v>10</v>
+      </c>
+      <c r="M10" s="4">
+        <v>7</v>
+      </c>
+      <c r="N10" s="4">
+        <v>1</v>
+      </c>
+      <c r="O10" s="4">
+        <v>2</v>
+      </c>
+      <c r="P10" s="4">
+        <v>70</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3295,11 +4039,35 @@
       <c r="G11" s="4">
         <v>20</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <v>10</v>
+      </c>
+      <c r="K11" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="L11" s="4">
+        <v>8</v>
+      </c>
+      <c r="M11" s="4">
+        <v>3</v>
+      </c>
+      <c r="N11" s="4">
+        <v>0</v>
+      </c>
+      <c r="O11" s="4">
+        <v>5</v>
+      </c>
+      <c r="P11" s="4">
+        <v>37.5</v>
+      </c>
+      <c r="Q11" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3321,11 +4089,35 @@
       <c r="G12" s="4">
         <v>60</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <v>11</v>
+      </c>
+      <c r="K12" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="L12" s="4">
+        <v>10</v>
+      </c>
+      <c r="M12" s="4">
+        <v>5</v>
+      </c>
+      <c r="N12" s="4">
+        <v>0</v>
+      </c>
+      <c r="O12" s="4">
+        <v>5</v>
+      </c>
+      <c r="P12" s="4">
+        <v>50</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>13</v>
       </c>
@@ -3347,11 +4139,35 @@
       <c r="G13" s="4">
         <v>66.7</v>
       </c>
-      <c r="H13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J13">
+        <v>13</v>
+      </c>
+      <c r="K13" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="L13" s="4">
+        <v>8</v>
+      </c>
+      <c r="M13" s="4">
+        <v>4</v>
+      </c>
+      <c r="N13" s="4">
+        <v>1</v>
+      </c>
+      <c r="O13" s="4">
+        <v>3</v>
+      </c>
+      <c r="P13" s="4">
+        <v>50</v>
+      </c>
+      <c r="Q13" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>14</v>
       </c>
@@ -3373,16 +4189,40 @@
       <c r="G14" s="4">
         <v>66.7</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <v>14</v>
+      </c>
+      <c r="K14" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="L14" s="4">
+        <v>6</v>
+      </c>
+      <c r="M14" s="4">
+        <v>4</v>
+      </c>
+      <c r="N14" s="4">
+        <v>0</v>
+      </c>
+      <c r="O14" s="4">
+        <v>2</v>
+      </c>
+      <c r="P14" s="4">
+        <v>66.7</v>
+      </c>
+      <c r="Q14" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>15</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C15" s="4">
         <v>3</v>
@@ -3399,16 +4239,40 @@
       <c r="G15" s="4">
         <v>0</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <v>15</v>
+      </c>
+      <c r="K15" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="L15" s="4">
+        <v>6</v>
+      </c>
+      <c r="M15" s="4">
+        <v>1</v>
+      </c>
+      <c r="N15" s="4">
+        <v>0</v>
+      </c>
+      <c r="O15" s="4">
+        <v>5</v>
+      </c>
+      <c r="P15" s="4">
+        <v>16.7</v>
+      </c>
+      <c r="Q15" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>16</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C16" s="4">
         <v>3</v>
@@ -3425,16 +4289,40 @@
       <c r="G16" s="4">
         <v>33.299999999999997</v>
       </c>
-      <c r="H16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H16" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J16">
+        <v>16</v>
+      </c>
+      <c r="K16" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="L16" s="4">
+        <v>6</v>
+      </c>
+      <c r="M16" s="4">
+        <v>2</v>
+      </c>
+      <c r="N16" s="4">
+        <v>1</v>
+      </c>
+      <c r="O16" s="4">
+        <v>3</v>
+      </c>
+      <c r="P16" s="4">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="Q16" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>17</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C17" s="4">
         <v>4</v>
@@ -3451,16 +4339,40 @@
       <c r="G17" s="2">
         <v>50</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J17">
+        <v>17</v>
+      </c>
+      <c r="K17" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="L17" s="4">
+        <v>8</v>
+      </c>
+      <c r="M17" s="4">
+        <v>5</v>
+      </c>
+      <c r="N17" s="4">
+        <v>2</v>
+      </c>
+      <c r="O17" s="4">
+        <v>1</v>
+      </c>
+      <c r="P17" s="4">
+        <v>62.5</v>
+      </c>
+      <c r="Q17" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>18</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C18" s="4">
         <v>4</v>
@@ -3477,16 +4389,40 @@
       <c r="G18" s="4">
         <v>0</v>
       </c>
-      <c r="H18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H18" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J18">
+        <v>18</v>
+      </c>
+      <c r="K18" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="L18" s="4">
+        <v>8</v>
+      </c>
+      <c r="M18" s="4">
+        <v>2</v>
+      </c>
+      <c r="N18" s="4">
+        <v>2</v>
+      </c>
+      <c r="O18" s="4">
+        <v>4</v>
+      </c>
+      <c r="P18" s="4">
+        <v>25</v>
+      </c>
+      <c r="Q18" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>19</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C19" s="4">
         <v>4</v>
@@ -3503,16 +4439,40 @@
       <c r="G19" s="4">
         <v>50</v>
       </c>
-      <c r="H19" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H19" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J19">
+        <v>19</v>
+      </c>
+      <c r="K19" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="L19" s="4">
+        <v>8</v>
+      </c>
+      <c r="M19" s="4">
+        <v>3</v>
+      </c>
+      <c r="N19" s="4">
+        <v>2</v>
+      </c>
+      <c r="O19" s="4">
+        <v>3</v>
+      </c>
+      <c r="P19" s="4">
+        <v>37.5</v>
+      </c>
+      <c r="Q19" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>20</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C20" s="4">
         <v>4</v>
@@ -3529,16 +4489,40 @@
       <c r="G20" s="4">
         <v>50</v>
       </c>
-      <c r="H20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H20" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J20">
+        <v>20</v>
+      </c>
+      <c r="K20" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="L20" s="4">
+        <v>8</v>
+      </c>
+      <c r="M20" s="4">
+        <v>3</v>
+      </c>
+      <c r="N20" s="4">
+        <v>1</v>
+      </c>
+      <c r="O20" s="4">
+        <v>4</v>
+      </c>
+      <c r="P20" s="4">
+        <v>37.5</v>
+      </c>
+      <c r="Q20" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>21</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C21" s="4">
         <v>4</v>
@@ -3555,16 +4539,40 @@
       <c r="G21" s="4">
         <v>50</v>
       </c>
-      <c r="H21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H21" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J21">
+        <v>21</v>
+      </c>
+      <c r="K21" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="L21" s="4">
+        <v>8</v>
+      </c>
+      <c r="M21" s="4">
+        <v>5</v>
+      </c>
+      <c r="N21" s="4">
+        <v>0</v>
+      </c>
+      <c r="O21" s="4">
+        <v>3</v>
+      </c>
+      <c r="P21" s="4">
+        <v>62.5</v>
+      </c>
+      <c r="Q21" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>22</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C22" s="2">
         <v>5</v>
@@ -3581,16 +4589,40 @@
       <c r="G22" s="4">
         <v>40</v>
       </c>
-      <c r="H22" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H22" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J22">
+        <v>22</v>
+      </c>
+      <c r="K22" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="L22" s="4">
+        <v>9</v>
+      </c>
+      <c r="M22" s="4">
+        <v>5</v>
+      </c>
+      <c r="N22" s="4">
+        <v>1</v>
+      </c>
+      <c r="O22" s="4">
+        <v>3</v>
+      </c>
+      <c r="P22" s="4">
+        <v>55.6</v>
+      </c>
+      <c r="Q22" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>23</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C23" s="2">
         <v>5</v>
@@ -3607,16 +4639,40 @@
       <c r="G23" s="4">
         <v>20</v>
       </c>
-      <c r="H23" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H23" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="J23">
+        <v>23</v>
+      </c>
+      <c r="K23" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="L23" s="4">
+        <v>9</v>
+      </c>
+      <c r="M23" s="4">
+        <v>2</v>
+      </c>
+      <c r="N23" s="4">
+        <v>2</v>
+      </c>
+      <c r="O23" s="4">
+        <v>5</v>
+      </c>
+      <c r="P23" s="4">
+        <v>22.2</v>
+      </c>
+      <c r="Q23" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>24</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C24" s="2">
         <v>5</v>
@@ -3633,16 +4689,40 @@
       <c r="G24" s="4">
         <v>40</v>
       </c>
-      <c r="H24" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H24" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J24">
+        <v>24</v>
+      </c>
+      <c r="K24" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="L24" s="4">
+        <v>9</v>
+      </c>
+      <c r="M24" s="4">
+        <v>3</v>
+      </c>
+      <c r="N24" s="4">
+        <v>1</v>
+      </c>
+      <c r="O24" s="4">
+        <v>5</v>
+      </c>
+      <c r="P24" s="4">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="Q24" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>25</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C25" s="2">
         <v>5</v>
@@ -3659,16 +4739,40 @@
       <c r="G25" s="4">
         <v>20</v>
       </c>
-      <c r="H25" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H25" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J25">
+        <v>25</v>
+      </c>
+      <c r="K25" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="L25" s="4">
+        <v>8</v>
+      </c>
+      <c r="M25" s="4">
+        <v>4</v>
+      </c>
+      <c r="N25" s="4">
+        <v>1</v>
+      </c>
+      <c r="O25" s="4">
+        <v>3</v>
+      </c>
+      <c r="P25" s="4">
+        <v>50</v>
+      </c>
+      <c r="Q25" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>26</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C26" s="2">
         <v>5</v>
@@ -3685,16 +4789,40 @@
       <c r="G26" s="4">
         <v>100</v>
       </c>
-      <c r="H26" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H26" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="J26">
+        <v>26</v>
+      </c>
+      <c r="K26" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="L26" s="4">
+        <v>9</v>
+      </c>
+      <c r="M26" s="4">
+        <v>6</v>
+      </c>
+      <c r="N26" s="4">
+        <v>0</v>
+      </c>
+      <c r="O26" s="4">
+        <v>3</v>
+      </c>
+      <c r="P26" s="4">
+        <v>66.7</v>
+      </c>
+      <c r="Q26" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>29</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C27" s="2">
         <v>5</v>
@@ -3711,16 +4839,40 @@
       <c r="G27" s="4">
         <v>40</v>
       </c>
-      <c r="H27" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H27" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J27">
+        <v>29</v>
+      </c>
+      <c r="K27" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="L27" s="4">
+        <v>9</v>
+      </c>
+      <c r="M27" s="4">
+        <v>4</v>
+      </c>
+      <c r="N27" s="4">
+        <v>1</v>
+      </c>
+      <c r="O27" s="4">
+        <v>4</v>
+      </c>
+      <c r="P27" s="4">
+        <v>44.4</v>
+      </c>
+      <c r="Q27" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>30</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>59</v>
+      <c r="B28" s="22" t="s">
+        <v>58</v>
       </c>
       <c r="C28" s="2">
         <v>2</v>
@@ -3737,16 +4889,40 @@
       <c r="G28" s="4">
         <v>50</v>
       </c>
-      <c r="H28" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H28" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J28">
+        <v>30</v>
+      </c>
+      <c r="K28" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="L28" s="4">
+        <v>5</v>
+      </c>
+      <c r="M28" s="4">
+        <v>2</v>
+      </c>
+      <c r="N28" s="4">
+        <v>0</v>
+      </c>
+      <c r="O28" s="4">
+        <v>3</v>
+      </c>
+      <c r="P28" s="4">
+        <v>40</v>
+      </c>
+      <c r="Q28" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>31</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>60</v>
+      <c r="B29" s="22" t="s">
+        <v>59</v>
       </c>
       <c r="C29" s="2">
         <v>2</v>
@@ -3763,16 +4939,40 @@
       <c r="G29" s="4">
         <v>50</v>
       </c>
-      <c r="H29" t="s">
+      <c r="H29" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J29">
+        <v>31</v>
+      </c>
+      <c r="K29" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="L29" s="4">
+        <v>5</v>
+      </c>
+      <c r="M29" s="4">
+        <v>1</v>
+      </c>
+      <c r="N29" s="4">
+        <v>0</v>
+      </c>
+      <c r="O29" s="4">
+        <v>4</v>
+      </c>
+      <c r="P29" s="4">
+        <v>20</v>
+      </c>
+      <c r="Q29" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>32</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>61</v>
+      <c r="B30" s="22" t="s">
+        <v>60</v>
       </c>
       <c r="C30" s="2">
         <v>2</v>
@@ -3789,8 +4989,32 @@
       <c r="G30" s="4">
         <v>50</v>
       </c>
-      <c r="H30" t="s">
-        <v>46</v>
+      <c r="H30" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J30">
+        <v>32</v>
+      </c>
+      <c r="K30" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="L30" s="4">
+        <v>5</v>
+      </c>
+      <c r="M30" s="4">
+        <v>3</v>
+      </c>
+      <c r="N30" s="4">
+        <v>0</v>
+      </c>
+      <c r="O30" s="4">
+        <v>2</v>
+      </c>
+      <c r="P30" s="4">
+        <v>60</v>
+      </c>
+      <c r="Q30" s="4" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>